<commit_message>
Updated DCR-Tempalte to include phone and fax options. Fixed some issues with datetype cells containing values when they did not. Fixed an issue with sections being created by access if a resource wasn't being assigned.
</commit_message>
<xml_diff>
--- a/DCR-Template.xlsx
+++ b/DCR-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DF8882-0208-4985-9D21-A78D295A8AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0251499A-19F2-4602-81CC-C48F05429202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="28680" yWindow="-9270" windowWidth="30960" windowHeight="16920" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Input Schema" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Drop Down List Values" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="208">
   <si>
     <t>Sections</t>
   </si>
@@ -871,6 +872,18 @@
   </si>
   <si>
     <t>CREM_C_RSP</t>
+  </si>
+  <si>
+    <t>Submittor Fax Number</t>
+  </si>
+  <si>
+    <t>Submittor Phone Number</t>
+  </si>
+  <si>
+    <t>Primary Contact Phone Number of the person who is submitting the Death Certificate Review Message</t>
+  </si>
+  <si>
+    <t>Primary Fax Address of the person who is submitting the Death Certificate Review Message</t>
   </si>
 </sst>
 </file>
@@ -2084,8 +2097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
   <dimension ref="A1:AU66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -2132,7 +2145,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="105.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" ht="105.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
@@ -2849,7 +2862,7 @@
       <c r="H51" s="42"/>
       <c r="I51" s="43"/>
     </row>
-    <row r="52" spans="1:47" s="44" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:47" s="44" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
       <c r="A52" s="60"/>
       <c r="B52" s="77" t="s">
         <v>109</v>
@@ -3349,10 +3362,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C559A218-9020-4822-8346-393500FE199B}">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
@@ -3444,72 +3457,74 @@
       <c r="H5" s="120"/>
       <c r="I5" s="115"/>
     </row>
-    <row r="6" spans="1:9" s="117" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" s="117" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A6" s="116"/>
       <c r="B6" s="118" t="s">
-        <v>178</v>
+        <v>205</v>
       </c>
       <c r="C6" s="119" t="s">
-        <v>180</v>
-      </c>
-      <c r="D6" s="143"/>
+        <v>206</v>
+      </c>
+      <c r="D6" s="120"/>
       <c r="E6" s="120"/>
       <c r="F6" s="120"/>
       <c r="G6" s="120"/>
       <c r="H6" s="120"/>
       <c r="I6" s="115"/>
     </row>
-    <row r="7" spans="1:9" s="138" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A7" s="134" t="s">
+    <row r="7" spans="1:9" s="117" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A7" s="116"/>
+      <c r="B7" s="118" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="119" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="115"/>
+    </row>
+    <row r="8" spans="1:9" s="117" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A8" s="116"/>
+      <c r="B8" s="118" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="119" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="143"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="120"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="115"/>
+    </row>
+    <row r="9" spans="1:9" s="138" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A9" s="134" t="s">
         <v>181</v>
       </c>
-      <c r="B7" s="135"/>
-      <c r="C7" s="136" t="s">
+      <c r="B9" s="135"/>
+      <c r="C9" s="136" t="s">
         <v>183</v>
       </c>
-      <c r="D7" s="137"/>
-      <c r="E7" s="137"/>
-      <c r="F7" s="137"/>
-      <c r="G7" s="137"/>
-      <c r="H7" s="137"/>
-      <c r="I7" s="137"/>
-    </row>
-    <row r="8" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="126"/>
-      <c r="B8" s="130" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" s="127" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="128"/>
-    </row>
-    <row r="9" spans="1:9" s="129" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A9" s="126"/>
-      <c r="B9" s="130" t="s">
-        <v>185</v>
-      </c>
-      <c r="C9" s="127" t="s">
-        <v>191</v>
-      </c>
-      <c r="D9" s="144"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="145"/>
-      <c r="G9" s="145"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="128"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="137"/>
+      <c r="F9" s="137"/>
+      <c r="G9" s="137"/>
+      <c r="H9" s="137"/>
+      <c r="I9" s="137"/>
     </row>
     <row r="10" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="126"/>
       <c r="B10" s="130" t="s">
-        <v>186</v>
-      </c>
-      <c r="C10" s="127"/>
+        <v>182</v>
+      </c>
+      <c r="C10" s="127" t="s">
+        <v>184</v>
+      </c>
       <c r="D10" s="131"/>
       <c r="E10" s="132"/>
       <c r="F10" s="132"/>
@@ -3517,23 +3532,25 @@
       <c r="H10" s="132"/>
       <c r="I10" s="128"/>
     </row>
-    <row r="11" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:9" s="129" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
       <c r="A11" s="126"/>
       <c r="B11" s="130" t="s">
-        <v>187</v>
-      </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="131"/>
-      <c r="E11" s="132"/>
-      <c r="F11" s="132"/>
-      <c r="G11" s="132"/>
+        <v>185</v>
+      </c>
+      <c r="C11" s="127" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="144"/>
+      <c r="E11" s="145"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="145"/>
       <c r="H11" s="132"/>
       <c r="I11" s="128"/>
     </row>
-    <row r="12" spans="1:9" s="129" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="126"/>
-      <c r="B12" s="133" t="s">
-        <v>188</v>
+      <c r="B12" s="130" t="s">
+        <v>186</v>
       </c>
       <c r="C12" s="127"/>
       <c r="D12" s="131"/>
@@ -3546,7 +3563,7 @@
     <row r="13" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A13" s="126"/>
       <c r="B13" s="130" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C13" s="127"/>
       <c r="D13" s="131"/>
@@ -3556,10 +3573,10 @@
       <c r="H13" s="132"/>
       <c r="I13" s="128"/>
     </row>
-    <row r="14" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:9" s="129" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
       <c r="A14" s="126"/>
-      <c r="B14" s="130" t="s">
-        <v>190</v>
+      <c r="B14" s="133" t="s">
+        <v>188</v>
       </c>
       <c r="C14" s="127"/>
       <c r="D14" s="131"/>
@@ -3572,49 +3589,73 @@
     <row r="15" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A15" s="126"/>
       <c r="B15" s="130" t="s">
-        <v>192</v>
-      </c>
-      <c r="C15" s="127" t="s">
-        <v>194</v>
-      </c>
-      <c r="D15" s="139"/>
-      <c r="E15" s="140"/>
-      <c r="F15" s="140"/>
-      <c r="G15" s="140"/>
-      <c r="H15" s="140"/>
+        <v>189</v>
+      </c>
+      <c r="C15" s="127"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="132"/>
+      <c r="G15" s="132"/>
+      <c r="H15" s="132"/>
       <c r="I15" s="128"/>
     </row>
     <row r="16" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A16" s="126"/>
       <c r="B16" s="130" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="127"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="132"/>
+      <c r="G16" s="132"/>
+      <c r="H16" s="132"/>
+      <c r="I16" s="128"/>
+    </row>
+    <row r="17" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="126"/>
+      <c r="B17" s="130" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="127" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="139"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="140"/>
+      <c r="H17" s="140"/>
+      <c r="I17" s="128"/>
+    </row>
+    <row r="18" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="126"/>
+      <c r="B18" s="130" t="s">
         <v>193</v>
       </c>
-      <c r="C16" s="127" t="s">
+      <c r="C18" s="127" t="s">
         <v>195</v>
       </c>
-      <c r="D16" s="141"/>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="140"/>
-      <c r="I16" s="128"/>
-    </row>
-    <row r="17" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="18" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="19" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="22" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="23" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="27" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="28" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="29" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="30" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="31" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="32" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="142"/>
+      <c r="F18" s="142"/>
+      <c r="G18" s="140"/>
+      <c r="H18" s="140"/>
+      <c r="I18" s="128"/>
+    </row>
+    <row r="19" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="21" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="33" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="34" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="35" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
@@ -3650,6 +3691,8 @@
     <row r="65" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="66" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="67" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="68" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="69" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -3660,19 +3703,19 @@
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>H9</xm:sqref>
+          <xm:sqref>H11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5D77A5B3-DC21-4455-8579-74CE8C477205}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H11</xm:sqref>
+          <xm:sqref>H13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{73E3C8C7-4C35-407D-BD90-B3CE9EDEF4AB}">
           <x14:formula1>
             <xm:f>'Drop Down List Values'!$B$2:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H10</xm:sqref>
+          <xm:sqref>H12</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B2DC812E-574B-475E-A423-79EFE715328F}">
           <x14:formula1>
@@ -3967,65 +4010,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
@@ -4039,7 +4023,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -4238,23 +4222,66 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4272,7 +4299,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4290,4 +4317,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Locatino of death address
</commit_message>
<xml_diff>
--- a/DCR-Template.xlsx
+++ b/DCR-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0251499A-19F2-4602-81CC-C48F05429202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E76048E-269C-42ED-9E96-09764B7BBBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-9270" windowWidth="30960" windowHeight="16920" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
@@ -18,7 +18,6 @@
     <sheet name="Drop Down List Values" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="212">
   <si>
     <t>Sections</t>
   </si>
@@ -197,12 +196,6 @@
     <t>Primary Address of Decedent's residence address. Multiple lines are supported.</t>
   </si>
   <si>
-    <t>Decedent Residence: city</t>
-  </si>
-  <si>
-    <t>Decedent Residence: county</t>
-  </si>
-  <si>
     <t>Decedent Residence: State, U.S. Territory or Canadian Province</t>
   </si>
   <si>
@@ -348,12 +341,6 @@
 * Tobacco Use Contribute to Death</t>
   </si>
   <si>
-    <t>Location of death</t>
-  </si>
-  <si>
-    <t>Full or partial address describing the location of death</t>
-  </si>
-  <si>
     <t>Location of Injury</t>
   </si>
   <si>
@@ -651,12 +638,6 @@
   </si>
   <si>
     <t>Medical Examiner</t>
-  </si>
-  <si>
-    <t>This section describes the Medical Examiners Office which processed this case</t>
-  </si>
-  <si>
-    <t>This Excel File can be imported into RAVEN2.0; converting into FHIR and importing into RAVEN. This tab describes the baseline input used.</t>
   </si>
   <si>
     <t>This Excel File can be imported into RAVEN2.0; converting into FHIR and importing into RAVEN. This tab describes the DCR specific data need for a Death Certificate Review, extending upon the "Base Input Schema"</t>
@@ -884,6 +865,36 @@
   </si>
   <si>
     <t>Primary Fax Address of the person who is submitting the Death Certificate Review Message</t>
+  </si>
+  <si>
+    <t>This Excel File can be imported into RAVEN2.0; converting into FHIR and importing into RAVEN</t>
+  </si>
+  <si>
+    <t>Decedent Residence: City</t>
+  </si>
+  <si>
+    <t>Decedent Residence: County</t>
+  </si>
+  <si>
+    <t>Location of Death: Street</t>
+  </si>
+  <si>
+    <t>Full or partial address describing the location of death. Multiple lines are supported.</t>
+  </si>
+  <si>
+    <t>Location of Death: City</t>
+  </si>
+  <si>
+    <t>Location of Death: County</t>
+  </si>
+  <si>
+    <t>Location of Death: State, U.S. Territory or Canadian Province</t>
+  </si>
+  <si>
+    <t>Location of Death: Postal Code</t>
+  </si>
+  <si>
+    <t>Location of Death: Country</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1236,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1270,10 +1281,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1363,10 +1370,6 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -1401,10 +1404,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1465,18 +1464,6 @@
     <xf numFmtId="0" fontId="7" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1553,14 +1540,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1754,12 +1733,12 @@
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1799,9 +1778,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1839,7 +1818,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1945,7 +1924,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2087,7 +2066,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2095,30 +2074,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:AU66"/>
+  <dimension ref="A1:AU71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="50" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="62" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="69" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="47" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" style="66" customWidth="1"/>
     <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2140,26 +2119,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="69" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="105.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="50" t="s">
+    <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C2" s="66" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="105.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="103" t="s">
+      <c r="B3" s="96"/>
+      <c r="C3" s="97" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="83" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="77" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3"/>
@@ -2170,41 +2149,41 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
-      <c r="A5" s="52"/>
-      <c r="B5" s="99" t="s">
+      <c r="A5" s="49"/>
+      <c r="B5" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="146"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="138"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="52"/>
-      <c r="B6" s="100" t="s">
+      <c r="A6" s="49"/>
+      <c r="B6" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="146"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
+      <c r="D6" s="138"/>
+      <c r="E6" s="138"/>
+      <c r="F6" s="138"/>
+      <c r="G6" s="138"/>
+      <c r="H6" s="138"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="85" t="s">
+      <c r="B7" s="61"/>
+      <c r="C7" s="79" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="7"/>
@@ -2215,14 +2194,14 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A8" s="54"/>
-      <c r="B8" s="70" t="s">
+      <c r="A8" s="51"/>
+      <c r="B8" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="147"/>
+      <c r="D8" s="139"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -2230,14 +2209,14 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="54"/>
-      <c r="B9" s="70" t="s">
+      <c r="A9" s="51"/>
+      <c r="B9" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="86" t="s">
+      <c r="C9" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="147"/>
+      <c r="D9" s="139"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -2245,14 +2224,14 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A10" s="54"/>
-      <c r="B10" s="70" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="147"/>
+      <c r="D10" s="139"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2260,14 +2239,14 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A11" s="54"/>
-      <c r="B11" s="71" t="s">
+      <c r="A11" s="51"/>
+      <c r="B11" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="86" t="s">
+      <c r="C11" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="147"/>
+      <c r="D11" s="139"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -2275,14 +2254,14 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="54"/>
-      <c r="B12" s="70" t="s">
+      <c r="A12" s="51"/>
+      <c r="B12" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="86" t="s">
+      <c r="C12" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="147"/>
+      <c r="D12" s="139"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -2290,14 +2269,14 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A13" s="54"/>
-      <c r="B13" s="70" t="s">
+      <c r="A13" s="51"/>
+      <c r="B13" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="86" t="s">
+      <c r="C13" s="80" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="147"/>
+      <c r="D13" s="139"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -2305,14 +2284,14 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="54"/>
-      <c r="B14" s="70" t="s">
+      <c r="A14" s="51"/>
+      <c r="B14" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="149"/>
+      <c r="D14" s="141"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -2320,12 +2299,12 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="54"/>
-      <c r="B15" s="70" t="s">
+      <c r="A15" s="51"/>
+      <c r="B15" s="67" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="86"/>
-      <c r="D15" s="147"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="139"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -2333,1030 +2312,1001 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A16" s="54"/>
-      <c r="B16" s="70" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="86" t="s">
+      <c r="C16" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="166"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
+      <c r="D16" s="158"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="54"/>
-      <c r="B17" s="70" t="s">
+      <c r="A17" s="51"/>
+      <c r="B17" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="C17" s="80"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="51"/>
+      <c r="B18" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C18" s="80"/>
+      <c r="D18" s="139"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+    </row>
+    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A19" s="51"/>
+      <c r="B19" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="86"/>
-      <c r="D17" s="167"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="109"/>
-      <c r="H17" s="109"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="54"/>
-      <c r="B18" s="70" t="s">
+      <c r="C19" s="80"/>
+      <c r="D19" s="139"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="51"/>
+      <c r="B20" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="86"/>
-      <c r="D18" s="167"/>
-      <c r="E18" s="109"/>
-      <c r="F18" s="109"/>
-      <c r="G18" s="109"/>
-      <c r="H18" s="109"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A19" s="54"/>
-      <c r="B19" s="72" t="s">
+      <c r="C20" s="80"/>
+      <c r="D20" s="139"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="10"/>
+    </row>
+    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="51"/>
+      <c r="B21" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="167"/>
-      <c r="E19" s="109"/>
-      <c r="F19" s="109"/>
-      <c r="G19" s="109"/>
-      <c r="H19" s="109"/>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="54"/>
-      <c r="B20" s="70" t="s">
+      <c r="C21" s="80"/>
+      <c r="D21" s="139"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" s="13" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A22" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="86"/>
-      <c r="D20" s="167"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="109"/>
-      <c r="G20" s="109"/>
-      <c r="H20" s="109"/>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="54"/>
-      <c r="B21" s="70" t="s">
+      <c r="B22" s="62"/>
+      <c r="C22" s="81" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="86"/>
-      <c r="D21" s="167"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="109"/>
-      <c r="G21" s="109"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" s="14" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A22" s="96" t="s">
+      <c r="D22" s="140"/>
+      <c r="E22" s="140"/>
+      <c r="F22" s="140"/>
+      <c r="G22" s="140"/>
+      <c r="H22" s="140"/>
+      <c r="I22" s="140"/>
+    </row>
+    <row r="23" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="52"/>
+      <c r="B23" s="95" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="65"/>
-      <c r="C22" s="87" t="s">
+      <c r="C23" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="148"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-    </row>
-    <row r="23" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="55"/>
-      <c r="B23" s="101" t="s">
+      <c r="D23" s="147"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="52"/>
+      <c r="B24" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="88" t="s">
+      <c r="C24" s="82" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="155"/>
-      <c r="E23" s="105"/>
-      <c r="F23" s="105"/>
-      <c r="G23" s="105"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="16"/>
-    </row>
-    <row r="24" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="55"/>
-      <c r="B24" s="101" t="s">
+      <c r="D24" s="143"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="52"/>
+      <c r="B25" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="88" t="s">
+      <c r="C25" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="151"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="16"/>
-    </row>
-    <row r="25" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="55"/>
-      <c r="B25" s="101" t="s">
+      <c r="D25" s="144"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="52"/>
+      <c r="B26" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="88" t="s">
+      <c r="C26" s="82" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="152"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="16"/>
-    </row>
-    <row r="26" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="55"/>
-      <c r="B26" s="101" t="s">
+      <c r="D26" s="144"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="27" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A27" s="52"/>
+      <c r="B27" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="88" t="s">
+      <c r="C27" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="152"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="16"/>
-    </row>
-    <row r="27" spans="1:9" s="17" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A27" s="55"/>
-      <c r="B27" s="101" t="s">
+      <c r="D27" s="144"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="15"/>
+    </row>
+    <row r="28" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A28" s="52"/>
+      <c r="B28" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C28" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="152"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="16"/>
-    </row>
-    <row r="28" spans="1:9" s="17" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A28" s="55"/>
-      <c r="B28" s="101" t="s">
+      <c r="D28" s="144"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="15"/>
+    </row>
+    <row r="29" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A29" s="52"/>
+      <c r="B29" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="88" t="s">
+      <c r="C29" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="152"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="16"/>
-    </row>
-    <row r="29" spans="1:9" s="17" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A29" s="55"/>
-      <c r="B29" s="101" t="s">
+      <c r="D29" s="144"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A30" s="52"/>
+      <c r="B30" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="88" t="s">
+      <c r="C30" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="152"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="16"/>
-    </row>
-    <row r="30" spans="1:9" s="17" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A30" s="55"/>
-      <c r="B30" s="101" t="s">
+      <c r="D30" s="142"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="15"/>
+    </row>
+    <row r="31" spans="1:9" s="16" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A31" s="52"/>
+      <c r="B31" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="88" t="s">
+      <c r="C31" s="82" t="s">
         <v>61</v>
       </c>
-      <c r="D30" s="150"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="16"/>
-    </row>
-    <row r="31" spans="1:9" s="17" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A31" s="55"/>
-      <c r="B31" s="101" t="s">
+      <c r="D31" s="144"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="15"/>
+    </row>
+    <row r="32" spans="1:9" s="16" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A32" s="52"/>
+      <c r="B32" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="88" t="s">
+      <c r="C32" s="82" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="152"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="16"/>
-    </row>
-    <row r="32" spans="1:9" s="17" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="55"/>
-      <c r="B32" s="73" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="88" t="s">
+      <c r="D32" s="145"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="15"/>
+    </row>
+    <row r="33" spans="1:9" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A33" s="52"/>
+      <c r="B33" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="D32" s="153"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="16"/>
-    </row>
-    <row r="33" spans="1:9" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A33" s="55"/>
-      <c r="B33" s="73" t="s">
+      <c r="C33" s="82" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="146"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="15"/>
+    </row>
+    <row r="34" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A34" s="52"/>
+      <c r="B34" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="88" t="s">
+      <c r="C34" s="82" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="154"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="16"/>
-    </row>
-    <row r="34" spans="1:9" s="17" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A34" s="55"/>
-      <c r="B34" s="73" t="s">
+      <c r="D34" s="148"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="101"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="15"/>
+    </row>
+    <row r="35" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="53"/>
+      <c r="B35" s="70" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="88" t="s">
+      <c r="C35" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="156"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="107"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="16"/>
-    </row>
-    <row r="35" spans="1:9" s="24" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="56"/>
-      <c r="B35" s="73" t="s">
+      <c r="D35" s="144"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="22"/>
+    </row>
+    <row r="36" spans="1:9" s="16" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A36" s="52"/>
+      <c r="B36" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C36" s="82" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="152"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="23"/>
-    </row>
-    <row r="36" spans="1:9" s="17" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A36" s="55"/>
-      <c r="B36" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="88" t="s">
+      <c r="D36" s="145"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="15"/>
+    </row>
+    <row r="37" spans="1:9" s="16" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A37" s="52"/>
+      <c r="B37" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="D36" s="153"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="16"/>
-    </row>
-    <row r="37" spans="1:9" s="17" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A37" s="55"/>
-      <c r="B37" s="73" t="s">
+      <c r="C37" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="145"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="15"/>
+    </row>
+    <row r="38" spans="1:9" s="25" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A38" s="91" t="s">
         <v>76</v>
       </c>
-      <c r="C37" s="88" t="s">
+      <c r="B38" s="63"/>
+      <c r="C38" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="D37" s="153"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="16"/>
-    </row>
-    <row r="38" spans="1:9" s="26" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="97" t="s">
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="24"/>
+    </row>
+    <row r="39" spans="1:9" s="28" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A39" s="54"/>
+      <c r="B39" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="C39" s="84" t="s">
+        <v>206</v>
+      </c>
+      <c r="D39" s="150"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="27"/>
+    </row>
+    <row r="40" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A40" s="54"/>
+      <c r="B40" s="71" t="s">
+        <v>207</v>
+      </c>
+      <c r="C40" s="84"/>
+      <c r="D40" s="150"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="27"/>
+    </row>
+    <row r="41" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A41" s="54"/>
+      <c r="B41" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="C41" s="84"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="27"/>
+    </row>
+    <row r="42" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A42" s="54"/>
+      <c r="B42" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="C42" s="84"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="27"/>
+    </row>
+    <row r="43" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A43" s="54"/>
+      <c r="B43" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="C43" s="84"/>
+      <c r="D43" s="150"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="27"/>
+    </row>
+    <row r="44" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A44" s="54"/>
+      <c r="B44" s="71" t="s">
+        <v>211</v>
+      </c>
+      <c r="C44" s="84"/>
+      <c r="D44" s="150"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="27"/>
+    </row>
+    <row r="45" spans="1:9" s="28" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A45" s="54"/>
+      <c r="B45" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="B38" s="66"/>
-      <c r="C38" s="89" t="s">
+      <c r="C45" s="84" t="s">
         <v>79</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-    </row>
-    <row r="39" spans="1:9" s="29" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A39" s="57"/>
-      <c r="B39" s="74" t="s">
+      <c r="D45" s="150"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="27"/>
+    </row>
+    <row r="46" spans="1:9" s="28" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A46" s="54"/>
+      <c r="B46" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="90" t="s">
+      <c r="C46" s="84" t="s">
         <v>81</v>
       </c>
-      <c r="D39" s="158"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="28"/>
-    </row>
-    <row r="40" spans="1:9" s="29" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A40" s="57"/>
-      <c r="B40" s="75" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="90" t="s">
+      <c r="D46" s="150"/>
+      <c r="E46" s="150"/>
+      <c r="F46" s="150"/>
+      <c r="G46" s="150"/>
+      <c r="H46" s="150"/>
+      <c r="I46" s="27"/>
+    </row>
+    <row r="47" spans="1:9" s="28" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A47" s="54"/>
+      <c r="B47" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="D40" s="158"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="28"/>
-    </row>
-    <row r="41" spans="1:9" s="29" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A41" s="57"/>
-      <c r="B41" s="74" t="s">
+      <c r="C47" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="C41" s="90" t="s">
+      <c r="D47" s="150"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="27"/>
+    </row>
+    <row r="48" spans="1:9" s="32" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A48" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="D41" s="158"/>
-      <c r="E41" s="80"/>
-      <c r="F41" s="80"/>
-      <c r="G41" s="80"/>
-      <c r="H41" s="80"/>
-      <c r="I41" s="28"/>
-    </row>
-    <row r="42" spans="1:9" s="29" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A42" s="57"/>
-      <c r="B42" s="98" t="s">
+      <c r="B48" s="64"/>
+      <c r="C48" s="85" t="s">
+        <v>86</v>
+      </c>
+      <c r="D48" s="151"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
+      <c r="H48" s="30"/>
+      <c r="I48" s="31"/>
+    </row>
+    <row r="49" spans="1:47" s="35" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A49" s="55"/>
+      <c r="B49" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="C42" s="90" t="s">
+      <c r="C49" s="86" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="158"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="28"/>
-    </row>
-    <row r="43" spans="1:9" s="33" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A43" s="104" t="s">
+      <c r="D49" s="152"/>
+      <c r="E49" s="33"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="34"/>
+    </row>
+    <row r="50" spans="1:47" s="35" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A50" s="55"/>
+      <c r="B50" s="73" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="67"/>
-      <c r="C43" s="91" t="s">
+      <c r="C50" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="D43" s="159"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="32"/>
-    </row>
-    <row r="44" spans="1:9" s="36" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A44" s="58"/>
-      <c r="B44" s="76" t="s">
+      <c r="D50" s="153"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="34"/>
+    </row>
+    <row r="51" spans="1:47" s="35" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A51" s="55"/>
+      <c r="B51" s="73" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="92" t="s">
+      <c r="C51" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="D44" s="160"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="35"/>
-    </row>
-    <row r="45" spans="1:9" s="36" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A45" s="58"/>
-      <c r="B45" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="C45" s="92" t="s">
+      <c r="D51" s="154"/>
+      <c r="E51" s="149"/>
+      <c r="F51" s="149"/>
+      <c r="G51" s="149"/>
+      <c r="H51" s="149"/>
+      <c r="I51" s="34"/>
+    </row>
+    <row r="52" spans="1:47" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A52" s="55"/>
+      <c r="B52" s="73" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="161"/>
-      <c r="E45" s="37"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37"/>
-      <c r="I45" s="35"/>
-    </row>
-    <row r="46" spans="1:9" s="36" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A46" s="58"/>
-      <c r="B46" s="76" t="s">
+      <c r="C52" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="92" t="s">
+      <c r="D52" s="155"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="34"/>
+    </row>
+    <row r="53" spans="1:47" s="35" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
+      <c r="A53" s="55"/>
+      <c r="B53" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="162"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="35"/>
-    </row>
-    <row r="47" spans="1:9" s="36" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A47" s="58"/>
-      <c r="B47" s="76" t="s">
+      <c r="C53" s="86" t="s">
+        <v>97</v>
+      </c>
+      <c r="D53" s="153"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="34"/>
+    </row>
+    <row r="54" spans="1:47" s="35" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A54" s="55"/>
+      <c r="B54" s="73" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="92" t="s">
+      <c r="C54" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="D47" s="163"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="35"/>
-    </row>
-    <row r="48" spans="1:9" s="36" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
-      <c r="A48" s="58"/>
-      <c r="B48" s="76" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" s="92" t="s">
+      <c r="D54" s="149"/>
+      <c r="E54" s="149"/>
+      <c r="F54" s="149"/>
+      <c r="G54" s="149"/>
+      <c r="H54" s="149"/>
+      <c r="I54" s="34"/>
+    </row>
+    <row r="55" spans="1:47" s="39" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A55" s="56" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="161"/>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="37"/>
-      <c r="I48" s="35"/>
-    </row>
-    <row r="49" spans="1:47" s="36" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A49" s="58"/>
-      <c r="B49" s="76" t="s">
+      <c r="B55" s="65"/>
+      <c r="C55" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="92" t="s">
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+    </row>
+    <row r="56" spans="1:47" s="42" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A56" s="57"/>
+      <c r="B56" s="74" t="s">
         <v>103</v>
       </c>
-      <c r="D49" s="157"/>
-      <c r="E49" s="38"/>
-      <c r="F49" s="38"/>
-      <c r="G49" s="38"/>
-      <c r="H49" s="38"/>
-      <c r="I49" s="35"/>
-    </row>
-    <row r="50" spans="1:47" s="41" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A50" s="59" t="s">
+      <c r="C56" s="88" t="s">
+        <v>104</v>
+      </c>
+      <c r="D56" s="156"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="41"/>
+    </row>
+    <row r="57" spans="1:47" s="42" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A57" s="57"/>
+      <c r="B57" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="68"/>
-      <c r="C50" s="93" t="s">
+      <c r="C57" s="88" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="40"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="40"/>
-      <c r="G50" s="40"/>
-      <c r="H50" s="40"/>
-      <c r="I50" s="40"/>
-    </row>
-    <row r="51" spans="1:47" s="44" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="60"/>
-      <c r="B51" s="77" t="s">
+      <c r="D57" s="156"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="41"/>
+    </row>
+    <row r="58" spans="1:47" s="42" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A58" s="57"/>
+      <c r="B58" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="94" t="s">
+      <c r="C58" s="88" t="s">
         <v>108</v>
       </c>
-      <c r="D51" s="164"/>
-      <c r="E51" s="42"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="42"/>
-      <c r="H51" s="42"/>
-      <c r="I51" s="43"/>
-    </row>
-    <row r="52" spans="1:47" s="44" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A52" s="60"/>
-      <c r="B52" s="77" t="s">
+      <c r="D58" s="156"/>
+      <c r="E58" s="156"/>
+      <c r="F58" s="156"/>
+      <c r="G58" s="156"/>
+      <c r="H58" s="156"/>
+      <c r="I58" s="57"/>
+    </row>
+    <row r="59" spans="1:47" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A59" s="57"/>
+      <c r="B59" s="74" t="s">
         <v>109</v>
       </c>
-      <c r="C52" s="94" t="s">
+      <c r="C59" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="D52" s="164"/>
-      <c r="E52" s="42"/>
-      <c r="F52" s="42"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="42"/>
-      <c r="I52" s="43"/>
-    </row>
-    <row r="53" spans="1:47" s="44" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A53" s="60"/>
-      <c r="B53" s="77" t="s">
+      <c r="D59" s="156"/>
+      <c r="E59" s="156"/>
+      <c r="F59" s="156"/>
+      <c r="G59" s="156"/>
+      <c r="H59" s="156"/>
+      <c r="I59" s="57"/>
+      <c r="J59" s="57"/>
+      <c r="K59" s="57"/>
+      <c r="L59" s="57"/>
+      <c r="M59" s="57"/>
+      <c r="N59" s="57"/>
+      <c r="O59" s="57"/>
+      <c r="P59" s="57"/>
+      <c r="Q59" s="57"/>
+      <c r="R59" s="57"/>
+      <c r="S59" s="57"/>
+      <c r="T59" s="57"/>
+      <c r="U59" s="57"/>
+      <c r="V59" s="57"/>
+      <c r="W59" s="57"/>
+      <c r="X59" s="57"/>
+      <c r="Y59" s="57"/>
+      <c r="Z59" s="57"/>
+      <c r="AA59" s="57"/>
+      <c r="AB59" s="57"/>
+      <c r="AC59" s="57"/>
+      <c r="AD59" s="57"/>
+      <c r="AE59" s="57"/>
+      <c r="AF59" s="57"/>
+      <c r="AG59" s="57"/>
+      <c r="AH59" s="57"/>
+      <c r="AI59" s="57"/>
+      <c r="AJ59" s="57"/>
+      <c r="AK59" s="57"/>
+      <c r="AL59" s="57"/>
+      <c r="AM59" s="57"/>
+      <c r="AN59" s="57"/>
+      <c r="AO59" s="57"/>
+      <c r="AP59" s="57"/>
+      <c r="AQ59" s="57"/>
+      <c r="AR59" s="57"/>
+      <c r="AS59" s="57"/>
+      <c r="AT59" s="57"/>
+      <c r="AU59" s="57"/>
+    </row>
+    <row r="60" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A60" s="57"/>
+      <c r="B60" s="74" t="s">
         <v>111</v>
       </c>
-      <c r="C53" s="94" t="s">
+      <c r="C60" s="88"/>
+      <c r="D60" s="156"/>
+      <c r="E60" s="156"/>
+      <c r="F60" s="156"/>
+      <c r="G60" s="156"/>
+      <c r="H60" s="156"/>
+      <c r="I60" s="57"/>
+      <c r="J60" s="57"/>
+      <c r="K60" s="57"/>
+      <c r="L60" s="57"/>
+      <c r="M60" s="57"/>
+      <c r="N60" s="57"/>
+      <c r="O60" s="57"/>
+      <c r="P60" s="57"/>
+      <c r="Q60" s="57"/>
+      <c r="R60" s="57"/>
+      <c r="S60" s="57"/>
+      <c r="T60" s="57"/>
+      <c r="U60" s="57"/>
+      <c r="V60" s="57"/>
+      <c r="W60" s="57"/>
+      <c r="X60" s="57"/>
+      <c r="Y60" s="57"/>
+      <c r="Z60" s="57"/>
+      <c r="AA60" s="57"/>
+      <c r="AB60" s="57"/>
+      <c r="AC60" s="57"/>
+      <c r="AD60" s="57"/>
+      <c r="AE60" s="57"/>
+      <c r="AF60" s="57"/>
+      <c r="AG60" s="57"/>
+      <c r="AH60" s="57"/>
+      <c r="AI60" s="57"/>
+      <c r="AJ60" s="57"/>
+      <c r="AK60" s="57"/>
+      <c r="AL60" s="57"/>
+      <c r="AM60" s="57"/>
+      <c r="AN60" s="57"/>
+      <c r="AO60" s="57"/>
+      <c r="AP60" s="57"/>
+      <c r="AQ60" s="57"/>
+      <c r="AR60" s="57"/>
+      <c r="AS60" s="57"/>
+      <c r="AT60" s="57"/>
+      <c r="AU60" s="57"/>
+    </row>
+    <row r="61" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A61" s="57"/>
+      <c r="B61" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="D53" s="164"/>
-      <c r="E53" s="81"/>
-      <c r="F53" s="81"/>
-      <c r="G53" s="81"/>
-      <c r="H53" s="81"/>
-      <c r="I53" s="60"/>
-    </row>
-    <row r="54" spans="1:47" s="45" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A54" s="60"/>
-      <c r="B54" s="77" t="s">
+      <c r="C61" s="88"/>
+      <c r="D61" s="156"/>
+      <c r="E61" s="156"/>
+      <c r="F61" s="156"/>
+      <c r="G61" s="156"/>
+      <c r="H61" s="156"/>
+      <c r="I61" s="57"/>
+      <c r="J61" s="57"/>
+      <c r="K61" s="57"/>
+      <c r="L61" s="57"/>
+      <c r="M61" s="57"/>
+      <c r="N61" s="57"/>
+      <c r="O61" s="57"/>
+      <c r="P61" s="57"/>
+      <c r="Q61" s="57"/>
+      <c r="R61" s="57"/>
+      <c r="S61" s="57"/>
+      <c r="T61" s="57"/>
+      <c r="U61" s="57"/>
+      <c r="V61" s="57"/>
+      <c r="W61" s="57"/>
+      <c r="X61" s="57"/>
+      <c r="Y61" s="57"/>
+      <c r="Z61" s="57"/>
+      <c r="AA61" s="57"/>
+      <c r="AB61" s="57"/>
+      <c r="AC61" s="57"/>
+      <c r="AD61" s="57"/>
+      <c r="AE61" s="57"/>
+      <c r="AF61" s="57"/>
+      <c r="AG61" s="57"/>
+      <c r="AH61" s="57"/>
+      <c r="AI61" s="57"/>
+      <c r="AJ61" s="57"/>
+      <c r="AK61" s="57"/>
+      <c r="AL61" s="57"/>
+      <c r="AM61" s="57"/>
+      <c r="AN61" s="57"/>
+      <c r="AO61" s="57"/>
+      <c r="AP61" s="57"/>
+      <c r="AQ61" s="57"/>
+      <c r="AR61" s="57"/>
+      <c r="AS61" s="57"/>
+      <c r="AT61" s="57"/>
+      <c r="AU61" s="57"/>
+    </row>
+    <row r="62" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A62" s="57"/>
+      <c r="B62" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="C54" s="94" t="s">
+      <c r="C62" s="88"/>
+      <c r="D62" s="156"/>
+      <c r="E62" s="156"/>
+      <c r="F62" s="156"/>
+      <c r="G62" s="156"/>
+      <c r="H62" s="156"/>
+      <c r="I62" s="57"/>
+      <c r="J62" s="57"/>
+      <c r="K62" s="57"/>
+      <c r="L62" s="57"/>
+      <c r="M62" s="57"/>
+      <c r="N62" s="57"/>
+      <c r="O62" s="57"/>
+      <c r="P62" s="57"/>
+      <c r="Q62" s="57"/>
+      <c r="R62" s="57"/>
+      <c r="S62" s="57"/>
+      <c r="T62" s="57"/>
+      <c r="U62" s="57"/>
+      <c r="V62" s="57"/>
+      <c r="W62" s="57"/>
+      <c r="X62" s="57"/>
+      <c r="Y62" s="57"/>
+      <c r="Z62" s="57"/>
+      <c r="AA62" s="57"/>
+      <c r="AB62" s="57"/>
+      <c r="AC62" s="57"/>
+      <c r="AD62" s="57"/>
+      <c r="AE62" s="57"/>
+      <c r="AF62" s="57"/>
+      <c r="AG62" s="57"/>
+      <c r="AH62" s="57"/>
+      <c r="AI62" s="57"/>
+      <c r="AJ62" s="57"/>
+      <c r="AK62" s="57"/>
+      <c r="AL62" s="57"/>
+      <c r="AM62" s="57"/>
+      <c r="AN62" s="57"/>
+      <c r="AO62" s="57"/>
+      <c r="AP62" s="57"/>
+      <c r="AQ62" s="57"/>
+      <c r="AR62" s="57"/>
+      <c r="AS62" s="57"/>
+      <c r="AT62" s="57"/>
+      <c r="AU62" s="57"/>
+    </row>
+    <row r="63" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A63" s="57"/>
+      <c r="B63" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="164"/>
-      <c r="E54" s="81"/>
-      <c r="F54" s="81"/>
-      <c r="G54" s="81"/>
-      <c r="H54" s="81"/>
-      <c r="I54" s="60"/>
-      <c r="J54" s="60"/>
-      <c r="K54" s="60"/>
-      <c r="L54" s="60"/>
-      <c r="M54" s="60"/>
-      <c r="N54" s="60"/>
-      <c r="O54" s="60"/>
-      <c r="P54" s="60"/>
-      <c r="Q54" s="60"/>
-      <c r="R54" s="60"/>
-      <c r="S54" s="60"/>
-      <c r="T54" s="60"/>
-      <c r="U54" s="60"/>
-      <c r="V54" s="60"/>
-      <c r="W54" s="60"/>
-      <c r="X54" s="60"/>
-      <c r="Y54" s="60"/>
-      <c r="Z54" s="60"/>
-      <c r="AA54" s="60"/>
-      <c r="AB54" s="60"/>
-      <c r="AC54" s="60"/>
-      <c r="AD54" s="60"/>
-      <c r="AE54" s="60"/>
-      <c r="AF54" s="60"/>
-      <c r="AG54" s="60"/>
-      <c r="AH54" s="60"/>
-      <c r="AI54" s="60"/>
-      <c r="AJ54" s="60"/>
-      <c r="AK54" s="60"/>
-      <c r="AL54" s="60"/>
-      <c r="AM54" s="60"/>
-      <c r="AN54" s="60"/>
-      <c r="AO54" s="60"/>
-      <c r="AP54" s="60"/>
-      <c r="AQ54" s="60"/>
-      <c r="AR54" s="60"/>
-      <c r="AS54" s="60"/>
-      <c r="AT54" s="60"/>
-      <c r="AU54" s="60"/>
-    </row>
-    <row r="55" spans="1:47" s="48" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A55" s="60"/>
-      <c r="B55" s="77" t="s">
+      <c r="C63" s="88"/>
+      <c r="D63" s="156"/>
+      <c r="E63" s="156"/>
+      <c r="F63" s="156"/>
+      <c r="G63" s="156"/>
+      <c r="H63" s="156"/>
+      <c r="I63" s="57"/>
+      <c r="J63" s="57"/>
+      <c r="K63" s="57"/>
+      <c r="L63" s="57"/>
+      <c r="M63" s="57"/>
+      <c r="N63" s="57"/>
+      <c r="O63" s="57"/>
+      <c r="P63" s="57"/>
+      <c r="Q63" s="57"/>
+      <c r="R63" s="57"/>
+      <c r="S63" s="57"/>
+      <c r="T63" s="57"/>
+      <c r="U63" s="57"/>
+      <c r="V63" s="57"/>
+      <c r="W63" s="57"/>
+      <c r="X63" s="57"/>
+      <c r="Y63" s="57"/>
+      <c r="Z63" s="57"/>
+      <c r="AA63" s="57"/>
+      <c r="AB63" s="57"/>
+      <c r="AC63" s="57"/>
+      <c r="AD63" s="57"/>
+      <c r="AE63" s="57"/>
+      <c r="AF63" s="57"/>
+      <c r="AG63" s="57"/>
+      <c r="AH63" s="57"/>
+      <c r="AI63" s="57"/>
+      <c r="AJ63" s="57"/>
+      <c r="AK63" s="57"/>
+      <c r="AL63" s="57"/>
+      <c r="AM63" s="57"/>
+      <c r="AN63" s="57"/>
+      <c r="AO63" s="57"/>
+      <c r="AP63" s="57"/>
+      <c r="AQ63" s="57"/>
+      <c r="AR63" s="57"/>
+      <c r="AS63" s="57"/>
+      <c r="AT63" s="57"/>
+      <c r="AU63" s="57"/>
+    </row>
+    <row r="64" spans="1:47" s="106" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A64" s="102" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="103"/>
+      <c r="C64" s="104"/>
+      <c r="D64" s="105"/>
+      <c r="E64" s="105"/>
+      <c r="F64" s="105"/>
+      <c r="G64" s="105"/>
+      <c r="H64" s="105"/>
+      <c r="I64" s="105"/>
+    </row>
+    <row r="65" spans="1:9" s="46" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A65" s="58"/>
+      <c r="B65" s="75" t="s">
         <v>115</v>
       </c>
-      <c r="C55" s="94"/>
-      <c r="D55" s="164"/>
-      <c r="E55" s="81"/>
-      <c r="F55" s="81"/>
-      <c r="G55" s="81"/>
-      <c r="H55" s="81"/>
-      <c r="I55" s="60"/>
-      <c r="J55" s="60"/>
-      <c r="K55" s="60"/>
-      <c r="L55" s="60"/>
-      <c r="M55" s="60"/>
-      <c r="N55" s="60"/>
-      <c r="O55" s="60"/>
-      <c r="P55" s="60"/>
-      <c r="Q55" s="60"/>
-      <c r="R55" s="60"/>
-      <c r="S55" s="60"/>
-      <c r="T55" s="60"/>
-      <c r="U55" s="60"/>
-      <c r="V55" s="60"/>
-      <c r="W55" s="60"/>
-      <c r="X55" s="60"/>
-      <c r="Y55" s="60"/>
-      <c r="Z55" s="60"/>
-      <c r="AA55" s="60"/>
-      <c r="AB55" s="60"/>
-      <c r="AC55" s="60"/>
-      <c r="AD55" s="60"/>
-      <c r="AE55" s="60"/>
-      <c r="AF55" s="60"/>
-      <c r="AG55" s="60"/>
-      <c r="AH55" s="60"/>
-      <c r="AI55" s="60"/>
-      <c r="AJ55" s="60"/>
-      <c r="AK55" s="60"/>
-      <c r="AL55" s="60"/>
-      <c r="AM55" s="60"/>
-      <c r="AN55" s="60"/>
-      <c r="AO55" s="60"/>
-      <c r="AP55" s="60"/>
-      <c r="AQ55" s="60"/>
-      <c r="AR55" s="60"/>
-      <c r="AS55" s="60"/>
-      <c r="AT55" s="60"/>
-      <c r="AU55" s="60"/>
-    </row>
-    <row r="56" spans="1:47" s="48" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="60"/>
-      <c r="B56" s="77" t="s">
+      <c r="C65" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="C56" s="94"/>
-      <c r="D56" s="164"/>
-      <c r="E56" s="81"/>
-      <c r="F56" s="81"/>
-      <c r="G56" s="81"/>
-      <c r="H56" s="81"/>
-      <c r="I56" s="60"/>
-      <c r="J56" s="60"/>
-      <c r="K56" s="60"/>
-      <c r="L56" s="60"/>
-      <c r="M56" s="60"/>
-      <c r="N56" s="60"/>
-      <c r="O56" s="60"/>
-      <c r="P56" s="60"/>
-      <c r="Q56" s="60"/>
-      <c r="R56" s="60"/>
-      <c r="S56" s="60"/>
-      <c r="T56" s="60"/>
-      <c r="U56" s="60"/>
-      <c r="V56" s="60"/>
-      <c r="W56" s="60"/>
-      <c r="X56" s="60"/>
-      <c r="Y56" s="60"/>
-      <c r="Z56" s="60"/>
-      <c r="AA56" s="60"/>
-      <c r="AB56" s="60"/>
-      <c r="AC56" s="60"/>
-      <c r="AD56" s="60"/>
-      <c r="AE56" s="60"/>
-      <c r="AF56" s="60"/>
-      <c r="AG56" s="60"/>
-      <c r="AH56" s="60"/>
-      <c r="AI56" s="60"/>
-      <c r="AJ56" s="60"/>
-      <c r="AK56" s="60"/>
-      <c r="AL56" s="60"/>
-      <c r="AM56" s="60"/>
-      <c r="AN56" s="60"/>
-      <c r="AO56" s="60"/>
-      <c r="AP56" s="60"/>
-      <c r="AQ56" s="60"/>
-      <c r="AR56" s="60"/>
-      <c r="AS56" s="60"/>
-      <c r="AT56" s="60"/>
-      <c r="AU56" s="60"/>
-    </row>
-    <row r="57" spans="1:47" s="48" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="60"/>
-      <c r="B57" s="77" t="s">
+      <c r="D65" s="157"/>
+      <c r="E65" s="157"/>
+      <c r="F65" s="157"/>
+      <c r="G65" s="157"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="45"/>
+    </row>
+    <row r="66" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A66" s="58"/>
+      <c r="B66" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="C57" s="94"/>
-      <c r="D57" s="164"/>
-      <c r="E57" s="81"/>
-      <c r="F57" s="81"/>
-      <c r="G57" s="81"/>
-      <c r="H57" s="81"/>
-      <c r="I57" s="60"/>
-      <c r="J57" s="60"/>
-      <c r="K57" s="60"/>
-      <c r="L57" s="60"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="60"/>
-      <c r="O57" s="60"/>
-      <c r="P57" s="60"/>
-      <c r="Q57" s="60"/>
-      <c r="R57" s="60"/>
-      <c r="S57" s="60"/>
-      <c r="T57" s="60"/>
-      <c r="U57" s="60"/>
-      <c r="V57" s="60"/>
-      <c r="W57" s="60"/>
-      <c r="X57" s="60"/>
-      <c r="Y57" s="60"/>
-      <c r="Z57" s="60"/>
-      <c r="AA57" s="60"/>
-      <c r="AB57" s="60"/>
-      <c r="AC57" s="60"/>
-      <c r="AD57" s="60"/>
-      <c r="AE57" s="60"/>
-      <c r="AF57" s="60"/>
-      <c r="AG57" s="60"/>
-      <c r="AH57" s="60"/>
-      <c r="AI57" s="60"/>
-      <c r="AJ57" s="60"/>
-      <c r="AK57" s="60"/>
-      <c r="AL57" s="60"/>
-      <c r="AM57" s="60"/>
-      <c r="AN57" s="60"/>
-      <c r="AO57" s="60"/>
-      <c r="AP57" s="60"/>
-      <c r="AQ57" s="60"/>
-      <c r="AR57" s="60"/>
-      <c r="AS57" s="60"/>
-      <c r="AT57" s="60"/>
-      <c r="AU57" s="60"/>
-    </row>
-    <row r="58" spans="1:47" s="48" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="60"/>
-      <c r="B58" s="77" t="s">
+      <c r="C66" s="89"/>
+      <c r="D66" s="157"/>
+      <c r="E66" s="44"/>
+      <c r="F66" s="44"/>
+      <c r="G66" s="44"/>
+      <c r="H66" s="44"/>
+      <c r="I66" s="45"/>
+    </row>
+    <row r="67" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A67" s="58"/>
+      <c r="B67" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="C58" s="94"/>
-      <c r="D58" s="164"/>
-      <c r="E58" s="81"/>
-      <c r="F58" s="81"/>
-      <c r="G58" s="81"/>
-      <c r="H58" s="81"/>
-      <c r="I58" s="60"/>
-      <c r="J58" s="60"/>
-      <c r="K58" s="60"/>
-      <c r="L58" s="60"/>
-      <c r="M58" s="60"/>
-      <c r="N58" s="60"/>
-      <c r="O58" s="60"/>
-      <c r="P58" s="60"/>
-      <c r="Q58" s="60"/>
-      <c r="R58" s="60"/>
-      <c r="S58" s="60"/>
-      <c r="T58" s="60"/>
-      <c r="U58" s="60"/>
-      <c r="V58" s="60"/>
-      <c r="W58" s="60"/>
-      <c r="X58" s="60"/>
-      <c r="Y58" s="60"/>
-      <c r="Z58" s="60"/>
-      <c r="AA58" s="60"/>
-      <c r="AB58" s="60"/>
-      <c r="AC58" s="60"/>
-      <c r="AD58" s="60"/>
-      <c r="AE58" s="60"/>
-      <c r="AF58" s="60"/>
-      <c r="AG58" s="60"/>
-      <c r="AH58" s="60"/>
-      <c r="AI58" s="60"/>
-      <c r="AJ58" s="60"/>
-      <c r="AK58" s="60"/>
-      <c r="AL58" s="60"/>
-      <c r="AM58" s="60"/>
-      <c r="AN58" s="60"/>
-      <c r="AO58" s="60"/>
-      <c r="AP58" s="60"/>
-      <c r="AQ58" s="60"/>
-      <c r="AR58" s="60"/>
-      <c r="AS58" s="60"/>
-      <c r="AT58" s="60"/>
-      <c r="AU58" s="60"/>
-    </row>
-    <row r="59" spans="1:47" s="114" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A59" s="110" t="s">
-        <v>172</v>
-      </c>
-      <c r="B59" s="111"/>
-      <c r="C59" s="112" t="s">
-        <v>173</v>
-      </c>
-      <c r="H59" s="113"/>
-      <c r="I59" s="113"/>
-    </row>
-    <row r="60" spans="1:47" s="48" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A60" s="61"/>
-      <c r="B60" s="78" t="s">
+      <c r="C67" s="89"/>
+      <c r="D67" s="157"/>
+      <c r="E67" s="44"/>
+      <c r="F67" s="44"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="44"/>
+      <c r="I67" s="45"/>
+    </row>
+    <row r="68" spans="1:9" s="46" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+      <c r="A68" s="58"/>
+      <c r="B68" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="C60" s="95" t="s">
+      <c r="C68" s="89"/>
+      <c r="D68" s="157"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="44"/>
+      <c r="G68" s="44"/>
+      <c r="H68" s="44"/>
+      <c r="I68" s="45"/>
+    </row>
+    <row r="69" spans="1:9" s="46" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A69" s="58"/>
+      <c r="B69" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="D60" s="165"/>
-      <c r="E60" s="82"/>
-      <c r="F60" s="82"/>
-      <c r="G60" s="82"/>
-      <c r="H60" s="46"/>
-      <c r="I60" s="47"/>
-    </row>
-    <row r="61" spans="1:47" s="48" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="61"/>
-      <c r="B61" s="78" t="s">
+      <c r="C69" s="89"/>
+      <c r="D69" s="157"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="44"/>
+      <c r="H69" s="44"/>
+      <c r="I69" s="45"/>
+    </row>
+    <row r="70" spans="1:9" s="46" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A70" s="58"/>
+      <c r="B70" s="75" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="95"/>
-      <c r="D61" s="165"/>
-      <c r="E61" s="82"/>
-      <c r="F61" s="82"/>
-      <c r="G61" s="82"/>
-      <c r="H61" s="46"/>
-      <c r="I61" s="47"/>
-    </row>
-    <row r="62" spans="1:47" s="48" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="61"/>
-      <c r="B62" s="78" t="s">
+      <c r="C70" s="89" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="95"/>
-      <c r="D62" s="165"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="46"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="47"/>
-    </row>
-    <row r="63" spans="1:47" s="48" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A63" s="61"/>
-      <c r="B63" s="79" t="s">
+      <c r="D70" s="157"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="44"/>
+      <c r="I70" s="45"/>
+    </row>
+    <row r="71" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A71" s="58"/>
+      <c r="B71" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="C63" s="95"/>
-      <c r="D63" s="165"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
-      <c r="I63" s="47"/>
-    </row>
-    <row r="64" spans="1:47" s="48" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A64" s="61"/>
-      <c r="B64" s="79" t="s">
+      <c r="C71" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="C64" s="95"/>
-      <c r="D64" s="165"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="46"/>
-      <c r="G64" s="46"/>
-      <c r="H64" s="46"/>
-      <c r="I64" s="47"/>
-    </row>
-    <row r="65" spans="1:9" s="48" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A65" s="61"/>
-      <c r="B65" s="78" t="s">
-        <v>125</v>
-      </c>
-      <c r="C65" s="95" t="s">
-        <v>126</v>
-      </c>
-      <c r="D65" s="165"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="46"/>
-      <c r="G65" s="46"/>
-      <c r="H65" s="46"/>
-      <c r="I65" s="47"/>
-    </row>
-    <row r="66" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="61"/>
-      <c r="B66" s="78" t="s">
-        <v>127</v>
-      </c>
-      <c r="C66" s="95" t="s">
-        <v>128</v>
-      </c>
-      <c r="D66" s="165"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="46"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="47"/>
+      <c r="D71" s="157"/>
+      <c r="E71" s="44"/>
+      <c r="F71" s="44"/>
+      <c r="G71" s="44"/>
+      <c r="H71" s="44"/>
+      <c r="I71" s="45"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2560A1C6-3FEA-4452-84E2-D4BC7FEE35BC}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$B$2:$B$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H10 D10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6714C258-4BD2-45CC-BA09-55489A06314D}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$C$2:$C$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H11 D11</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6EE5A822-FD38-4314-981B-8ED84EDD69EC}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$E$2:$E$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>H32</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DC01C7B9-BA05-42AD-B9A9-F2FD4557F0F1}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$F$2:$F$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>H36</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7CC0EF60-AEB4-4234-B37C-4A02B7E2DE3B}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$G$2:$G$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H37</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D99AC123-497D-47BE-A346-1D3330E13BAC}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$I$2:$I$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>H42 D42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2388147A-1FAB-42AF-9190-67DEDF83A4EA}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$J$2:$J$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>H49 D49</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{093E1169-867D-4A32-AC3C-DC58C26E3C39}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$M$2:$M$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H66</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{33A578CF-33CA-4B41-B2C5-7541E5042FC9}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$A$2:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>H9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{77990685-A35A-4CD2-A1C0-E931CAE699E2}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$L$2:$L$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>H41 D41</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E0C755F2-6856-4118-9F77-76F8475243FA}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E46:G46 E10:G11 D32:G32 D36:G37 E41:G42 E49:G49</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{42CF6A8A-0F3A-4568-B9E2-BCEDE7FAF2A2}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E9:G9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{60A55124-4F75-458A-9282-7620480C2BA3}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$A$1:$A$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>D9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4462E45F-28EE-7C43-87D7-6FE56EB1D45E}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!$K$2:$K$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>D46</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{38BD6F45-E1D6-4C47-97BB-112AE837004E}">
-          <x14:formula1>
-            <xm:f>'Drop Down List Values'!O2:O4</xm:f>
-          </x14:formula1>
-          <xm:sqref>H46</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3370,22 +3320,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="50" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="62" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="69" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="47" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="59" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" style="66" customWidth="1"/>
     <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3408,239 +3358,239 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.5">
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="66" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="115" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A3" s="113" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="116"/>
+      <c r="C3" s="117" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="114"/>
+    </row>
+    <row r="4" spans="1:9" s="109" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.5">
+      <c r="A4" s="108"/>
+      <c r="B4" s="110" t="s">
+        <v>190</v>
+      </c>
+      <c r="C4" s="111" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="107"/>
+    </row>
+    <row r="5" spans="1:9" s="109" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A5" s="108"/>
+      <c r="B5" s="110" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="111" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="107"/>
+    </row>
+    <row r="6" spans="1:9" s="109" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A6" s="108"/>
+      <c r="B6" s="110" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="111" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="112"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="107"/>
+    </row>
+    <row r="7" spans="1:9" s="109" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A7" s="108"/>
+      <c r="B7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="C7" s="111" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="112"/>
+      <c r="E7" s="112"/>
+      <c r="F7" s="112"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="107"/>
+    </row>
+    <row r="8" spans="1:9" s="109" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A8" s="108"/>
+      <c r="B8" s="110" t="s">
+        <v>172</v>
+      </c>
+      <c r="C8" s="111" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="135"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="112"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="107"/>
+    </row>
+    <row r="9" spans="1:9" s="130" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A9" s="126" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="123" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A3" s="121" t="s">
+      <c r="B9" s="127"/>
+      <c r="C9" s="128" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="129"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="129"/>
+      <c r="G9" s="129"/>
+      <c r="H9" s="129"/>
+      <c r="I9" s="129"/>
+    </row>
+    <row r="10" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="118"/>
+      <c r="B10" s="122" t="s">
         <v>176</v>
       </c>
-      <c r="B3" s="124"/>
-      <c r="C3" s="125" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-    </row>
-    <row r="4" spans="1:9" s="117" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.5">
-      <c r="A4" s="116"/>
-      <c r="B4" s="118" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="119" t="s">
-        <v>197</v>
-      </c>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="G4" s="120"/>
-      <c r="H4" s="120"/>
-      <c r="I4" s="115"/>
-    </row>
-    <row r="5" spans="1:9" s="117" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A5" s="116"/>
-      <c r="B5" s="118" t="s">
-        <v>177</v>
-      </c>
-      <c r="C5" s="119" t="s">
+      <c r="C10" s="119" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="123"/>
+      <c r="E10" s="124"/>
+      <c r="F10" s="124"/>
+      <c r="G10" s="124"/>
+      <c r="H10" s="124"/>
+      <c r="I10" s="120"/>
+    </row>
+    <row r="11" spans="1:9" s="121" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A11" s="118"/>
+      <c r="B11" s="122" t="s">
         <v>179</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
-      <c r="G5" s="120"/>
-      <c r="H5" s="120"/>
-      <c r="I5" s="115"/>
-    </row>
-    <row r="6" spans="1:9" s="117" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A6" s="116"/>
-      <c r="B6" s="118" t="s">
-        <v>205</v>
-      </c>
-      <c r="C6" s="119" t="s">
-        <v>206</v>
-      </c>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
-      <c r="G6" s="120"/>
-      <c r="H6" s="120"/>
-      <c r="I6" s="115"/>
-    </row>
-    <row r="7" spans="1:9" s="117" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A7" s="116"/>
-      <c r="B7" s="118" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" s="119" t="s">
-        <v>207</v>
-      </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="115"/>
-    </row>
-    <row r="8" spans="1:9" s="117" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A8" s="116"/>
-      <c r="B8" s="118" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" s="119" t="s">
+      <c r="C11" s="119" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="136"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="124"/>
+      <c r="I11" s="120"/>
+    </row>
+    <row r="12" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="118"/>
+      <c r="B12" s="122" t="s">
         <v>180</v>
       </c>
-      <c r="D8" s="143"/>
-      <c r="E8" s="120"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="120"/>
-      <c r="H8" s="120"/>
-      <c r="I8" s="115"/>
-    </row>
-    <row r="9" spans="1:9" s="138" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A9" s="134" t="s">
+      <c r="C12" s="119"/>
+      <c r="D12" s="123"/>
+      <c r="E12" s="124"/>
+      <c r="F12" s="124"/>
+      <c r="G12" s="124"/>
+      <c r="H12" s="124"/>
+      <c r="I12" s="120"/>
+    </row>
+    <row r="13" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="118"/>
+      <c r="B13" s="122" t="s">
         <v>181</v>
       </c>
-      <c r="B9" s="135"/>
-      <c r="C9" s="136" t="s">
+      <c r="C13" s="119"/>
+      <c r="D13" s="123"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="124"/>
+      <c r="G13" s="124"/>
+      <c r="H13" s="124"/>
+      <c r="I13" s="120"/>
+    </row>
+    <row r="14" spans="1:9" s="121" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+      <c r="A14" s="118"/>
+      <c r="B14" s="125" t="s">
+        <v>182</v>
+      </c>
+      <c r="C14" s="119"/>
+      <c r="D14" s="123"/>
+      <c r="E14" s="124"/>
+      <c r="F14" s="124"/>
+      <c r="G14" s="124"/>
+      <c r="H14" s="124"/>
+      <c r="I14" s="120"/>
+    </row>
+    <row r="15" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="118"/>
+      <c r="B15" s="122" t="s">
         <v>183</v>
       </c>
-      <c r="D9" s="137"/>
-      <c r="E9" s="137"/>
-      <c r="F9" s="137"/>
-      <c r="G9" s="137"/>
-      <c r="H9" s="137"/>
-      <c r="I9" s="137"/>
-    </row>
-    <row r="10" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="126"/>
-      <c r="B10" s="130" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" s="127" t="s">
+      <c r="C15" s="119"/>
+      <c r="D15" s="123"/>
+      <c r="E15" s="124"/>
+      <c r="F15" s="124"/>
+      <c r="G15" s="124"/>
+      <c r="H15" s="124"/>
+      <c r="I15" s="120"/>
+    </row>
+    <row r="16" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="118"/>
+      <c r="B16" s="122" t="s">
         <v>184</v>
       </c>
-      <c r="D10" s="131"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="128"/>
-    </row>
-    <row r="11" spans="1:9" s="129" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A11" s="126"/>
-      <c r="B11" s="130" t="s">
-        <v>185</v>
-      </c>
-      <c r="C11" s="127" t="s">
-        <v>191</v>
-      </c>
-      <c r="D11" s="144"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="145"/>
-      <c r="G11" s="145"/>
-      <c r="H11" s="132"/>
-      <c r="I11" s="128"/>
-    </row>
-    <row r="12" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="126"/>
-      <c r="B12" s="130" t="s">
+      <c r="C16" s="119"/>
+      <c r="D16" s="123"/>
+      <c r="E16" s="124"/>
+      <c r="F16" s="124"/>
+      <c r="G16" s="124"/>
+      <c r="H16" s="124"/>
+      <c r="I16" s="120"/>
+    </row>
+    <row r="17" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="118"/>
+      <c r="B17" s="122" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="127"/>
-      <c r="D12" s="131"/>
-      <c r="E12" s="132"/>
-      <c r="F12" s="132"/>
-      <c r="G12" s="132"/>
-      <c r="H12" s="132"/>
-      <c r="I12" s="128"/>
-    </row>
-    <row r="13" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="126"/>
-      <c r="B13" s="130" t="s">
+      <c r="C17" s="119" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="132"/>
+      <c r="H17" s="132"/>
+      <c r="I17" s="120"/>
+    </row>
+    <row r="18" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="118"/>
+      <c r="B18" s="122" t="s">
         <v>187</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="131"/>
-      <c r="E13" s="132"/>
-      <c r="F13" s="132"/>
-      <c r="G13" s="132"/>
-      <c r="H13" s="132"/>
-      <c r="I13" s="128"/>
-    </row>
-    <row r="14" spans="1:9" s="129" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="126"/>
-      <c r="B14" s="133" t="s">
-        <v>188</v>
-      </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="131"/>
-      <c r="E14" s="132"/>
-      <c r="F14" s="132"/>
-      <c r="G14" s="132"/>
-      <c r="H14" s="132"/>
-      <c r="I14" s="128"/>
-    </row>
-    <row r="15" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="126"/>
-      <c r="B15" s="130" t="s">
+      <c r="C18" s="119" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="127"/>
-      <c r="D15" s="131"/>
-      <c r="E15" s="132"/>
-      <c r="F15" s="132"/>
-      <c r="G15" s="132"/>
-      <c r="H15" s="132"/>
-      <c r="I15" s="128"/>
-    </row>
-    <row r="16" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="126"/>
-      <c r="B16" s="130" t="s">
-        <v>190</v>
-      </c>
-      <c r="C16" s="127"/>
-      <c r="D16" s="131"/>
-      <c r="E16" s="132"/>
-      <c r="F16" s="132"/>
-      <c r="G16" s="132"/>
-      <c r="H16" s="132"/>
-      <c r="I16" s="128"/>
-    </row>
-    <row r="17" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="126"/>
-      <c r="B17" s="130" t="s">
-        <v>192</v>
-      </c>
-      <c r="C17" s="127" t="s">
-        <v>194</v>
-      </c>
-      <c r="D17" s="139"/>
-      <c r="E17" s="140"/>
-      <c r="F17" s="140"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="140"/>
-      <c r="I17" s="128"/>
-    </row>
-    <row r="18" spans="1:9" s="129" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="126"/>
-      <c r="B18" s="130" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="127" t="s">
-        <v>195</v>
-      </c>
-      <c r="D18" s="141"/>
-      <c r="E18" s="142"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="140"/>
-      <c r="I18" s="128"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="134"/>
+      <c r="F18" s="134"/>
+      <c r="G18" s="132"/>
+      <c r="H18" s="132"/>
+      <c r="I18" s="120"/>
     </row>
     <row r="19" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
@@ -3763,48 +3713,48 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
         <v>130</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
         <v>131</v>
       </c>
-      <c r="E1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="L1" t="s">
         <v>132</v>
       </c>
-      <c r="G1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" t="s">
-        <v>133</v>
-      </c>
-      <c r="I1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" t="s">
-        <v>136</v>
-      </c>
       <c r="M1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="N1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -3813,157 +3763,157 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F2" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" t="s">
+        <v>138</v>
+      </c>
+      <c r="K2" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" t="s">
         <v>139</v>
       </c>
-      <c r="F2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G2" t="s">
-        <v>141</v>
-      </c>
-      <c r="H2" t="s">
-        <v>140</v>
-      </c>
-      <c r="I2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J2" t="s">
-        <v>142</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" t="s">
-        <v>143</v>
-      </c>
       <c r="M2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="N2" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" t="s">
+        <v>144</v>
+      </c>
+      <c r="L3" t="s">
         <v>145</v>
       </c>
-      <c r="D3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="M3" t="s">
         <v>146</v>
       </c>
-      <c r="H3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J3" t="s">
-        <v>147</v>
-      </c>
-      <c r="K3" t="s">
-        <v>148</v>
-      </c>
-      <c r="L3" t="s">
-        <v>149</v>
-      </c>
-      <c r="M3" t="s">
-        <v>150</v>
-      </c>
       <c r="N3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" t="s">
         <v>151</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" t="s">
         <v>152</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" t="s">
+        <v>148</v>
+      </c>
+      <c r="I4" t="s">
         <v>153</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
         <v>154</v>
       </c>
-      <c r="E4" t="s">
+      <c r="K4" t="s">
         <v>155</v>
       </c>
-      <c r="F4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>156</v>
       </c>
-      <c r="H4" t="s">
-        <v>152</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>157</v>
       </c>
-      <c r="J4" t="s">
-        <v>158</v>
-      </c>
-      <c r="K4" t="s">
-        <v>159</v>
-      </c>
-      <c r="L4" t="s">
-        <v>160</v>
-      </c>
-      <c r="M4" t="s">
-        <v>161</v>
-      </c>
       <c r="N4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I5" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="J5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="N5" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -3971,36 +3921,36 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="L6" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N6" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="J7" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="L7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -4010,20 +3960,65 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
-      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
-      <Description>YVWEJ5DVYS2U-421999773-68</Description>
-    </_dlc_DocIdUrl>
-    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -4222,84 +4217,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
+      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
+      <Description>YVWEJ5DVYS2U-421999773-68</Description>
+    </_dlc_DocIdUrl>
+    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4319,18 +4267,20 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated templates to match new injury address structure.
</commit_message>
<xml_diff>
--- a/DCR-Template.xlsx
+++ b/DCR-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mriley7\workspace\raven-import-and-submit-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E76048E-269C-42ED-9E96-09764B7BBBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE25A5C-6F17-4CFF-ADB6-752314F8A397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9270" windowWidth="30960" windowHeight="16920" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7A50F290-1C75-487E-9806-F93553E4E7CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Base Input Schema" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="216">
   <si>
     <t>Sections</t>
   </si>
@@ -341,17 +341,7 @@
 * Tobacco Use Contribute to Death</t>
   </si>
   <si>
-    <t>Location of Injury</t>
-  </si>
-  <si>
-    <t>If an injury occurred, description of location, full, or partial address of the location of injury</t>
-  </si>
-  <si>
     <t>Pregnancy status</t>
-  </si>
-  <si>
-    <t>Was the decedent pregenant, and how close to term was the decedent?
-Accepted values are shown in the dropdown</t>
   </si>
   <si>
     <t>Not Applicable</t>
@@ -895,6 +885,27 @@
   </si>
   <si>
     <t>Location of Death: Country</t>
+  </si>
+  <si>
+    <t>Location of Injury: Street</t>
+  </si>
+  <si>
+    <t>Location of Injury: City</t>
+  </si>
+  <si>
+    <t>Location of Injury: County</t>
+  </si>
+  <si>
+    <t>Location of Injury: State, U.S. Territory or Canadian Province</t>
+  </si>
+  <si>
+    <t>Location of Injury: Postal Code</t>
+  </si>
+  <si>
+    <t>Location of Injury: Country</t>
+  </si>
+  <si>
+    <t>Full or partial address describing the location of injury. Multiple lines are supported.</t>
   </si>
 </sst>
 </file>
@@ -1236,7 +1247,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1340,9 +1351,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1739,6 +1747,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2074,30 +2093,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54CD1DC7-E143-4CF5-BEA9-4DABBAFFC7B0}">
-  <dimension ref="A1:AU71"/>
+  <dimension ref="A1:AU76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="C38" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="47" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="59" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="66" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" style="65" customWidth="1"/>
     <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -2120,25 +2139,25 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="23.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C2" s="66" t="s">
-        <v>202</v>
+      <c r="C2" s="65" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="105.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="97" t="s">
+      <c r="B3" s="95"/>
+      <c r="C3" s="96" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="34.799999999999997" thickTop="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="77" t="s">
+      <c r="B4" s="59"/>
+      <c r="C4" s="76" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="3"/>
@@ -2149,41 +2168,41 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" s="6" customFormat="1" ht="29.4" x14ac:dyDescent="0.5">
-      <c r="A5" s="49"/>
-      <c r="B5" s="93" t="s">
+      <c r="A5" s="48"/>
+      <c r="B5" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="138"/>
-      <c r="E5" s="138"/>
-      <c r="F5" s="138"/>
-      <c r="G5" s="138"/>
-      <c r="H5" s="138"/>
+      <c r="D5" s="137"/>
+      <c r="E5" s="137"/>
+      <c r="F5" s="137"/>
+      <c r="G5" s="137"/>
+      <c r="H5" s="137"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A6" s="49"/>
-      <c r="B6" s="94" t="s">
+      <c r="A6" s="48"/>
+      <c r="B6" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
-      <c r="F6" s="138"/>
-      <c r="G6" s="138"/>
-      <c r="H6" s="138"/>
+      <c r="D6" s="137"/>
+      <c r="E6" s="137"/>
+      <c r="F6" s="137"/>
+      <c r="G6" s="137"/>
+      <c r="H6" s="137"/>
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="8" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="79" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="78" t="s">
         <v>18</v>
       </c>
       <c r="D7" s="7"/>
@@ -2194,14 +2213,14 @@
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" s="11" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A8" s="51"/>
-      <c r="B8" s="67" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="139"/>
+      <c r="D8" s="138"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -2209,14 +2228,14 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A9" s="51"/>
-      <c r="B9" s="67" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="139"/>
+      <c r="D9" s="138"/>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
@@ -2224,14 +2243,14 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A10" s="51"/>
-      <c r="B10" s="67" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="139"/>
+      <c r="D10" s="138"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -2239,14 +2258,14 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" s="11" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A11" s="51"/>
-      <c r="B11" s="68" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="139"/>
+      <c r="D11" s="138"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -2254,14 +2273,14 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A12" s="51"/>
-      <c r="B12" s="67" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="80" t="s">
+      <c r="C12" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="139"/>
+      <c r="D12" s="138"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -2269,14 +2288,14 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" s="11" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A13" s="51"/>
-      <c r="B13" s="67" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="139"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -2284,14 +2303,14 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" s="11" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="51"/>
-      <c r="B14" s="67" t="s">
+      <c r="A14" s="50"/>
+      <c r="B14" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="80" t="s">
+      <c r="C14" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="141"/>
+      <c r="D14" s="140"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -2299,12 +2318,12 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="51"/>
-      <c r="B15" s="67" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="80"/>
-      <c r="D15" s="139"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="138"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
@@ -2312,27 +2331,27 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" s="11" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A16" s="51"/>
-      <c r="B16" s="67" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="158"/>
-      <c r="E16" s="159"/>
-      <c r="F16" s="159"/>
+      <c r="D16" s="157"/>
+      <c r="E16" s="158"/>
+      <c r="F16" s="158"/>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="51"/>
-      <c r="B17" s="67" t="s">
-        <v>203</v>
-      </c>
-      <c r="C17" s="80"/>
-      <c r="D17" s="139"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="66" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" s="79"/>
+      <c r="D17" s="138"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
@@ -2340,12 +2359,12 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="51"/>
-      <c r="B18" s="67" t="s">
-        <v>204</v>
-      </c>
-      <c r="C18" s="80"/>
-      <c r="D18" s="139"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="66" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" s="79"/>
+      <c r="D18" s="138"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
@@ -2353,12 +2372,12 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" s="11" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A19" s="51"/>
-      <c r="B19" s="69" t="s">
+      <c r="A19" s="50"/>
+      <c r="B19" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="139"/>
+      <c r="C19" s="79"/>
+      <c r="D19" s="138"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
@@ -2366,12 +2385,12 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="51"/>
-      <c r="B20" s="67" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="80"/>
-      <c r="D20" s="139"/>
+      <c r="C20" s="79"/>
+      <c r="D20" s="138"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
@@ -2379,12 +2398,12 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="51"/>
-      <c r="B21" s="67" t="s">
+      <c r="A21" s="50"/>
+      <c r="B21" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="80"/>
-      <c r="D21" s="139"/>
+      <c r="C21" s="79"/>
+      <c r="D21" s="138"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
@@ -2392,59 +2411,59 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" s="13" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A22" s="90" t="s">
+      <c r="A22" s="89" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="62"/>
-      <c r="C22" s="81" t="s">
+      <c r="B22" s="61"/>
+      <c r="C22" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="D22" s="140"/>
-      <c r="E22" s="140"/>
-      <c r="F22" s="140"/>
-      <c r="G22" s="140"/>
-      <c r="H22" s="140"/>
-      <c r="I22" s="140"/>
+      <c r="D22" s="139"/>
+      <c r="E22" s="139"/>
+      <c r="F22" s="139"/>
+      <c r="G22" s="139"/>
+      <c r="H22" s="139"/>
+      <c r="I22" s="139"/>
     </row>
     <row r="23" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="52"/>
-      <c r="B23" s="95" t="s">
+      <c r="A23" s="51"/>
+      <c r="B23" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="147"/>
-      <c r="E23" s="99"/>
-      <c r="F23" s="99"/>
-      <c r="G23" s="99"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="98"/>
       <c r="H23" s="14"/>
       <c r="I23" s="15"/>
     </row>
     <row r="24" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="52"/>
-      <c r="B24" s="95" t="s">
+      <c r="A24" s="51"/>
+      <c r="B24" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="82" t="s">
+      <c r="C24" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="143"/>
+      <c r="D24" s="142"/>
       <c r="E24" s="17"/>
-      <c r="F24" s="100"/>
+      <c r="F24" s="99"/>
       <c r="G24" s="17"/>
       <c r="H24" s="17"/>
       <c r="I24" s="15"/>
     </row>
     <row r="25" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="52"/>
-      <c r="B25" s="95" t="s">
+      <c r="A25" s="51"/>
+      <c r="B25" s="94" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="82" t="s">
+      <c r="C25" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="144"/>
+      <c r="D25" s="143"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
@@ -2452,14 +2471,14 @@
       <c r="I25" s="15"/>
     </row>
     <row r="26" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="52"/>
-      <c r="B26" s="95" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="82" t="s">
+      <c r="C26" s="81" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="144"/>
+      <c r="D26" s="143"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
@@ -2467,14 +2486,14 @@
       <c r="I26" s="15"/>
     </row>
     <row r="27" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A27" s="52"/>
-      <c r="B27" s="95" t="s">
+      <c r="A27" s="51"/>
+      <c r="B27" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="144"/>
+      <c r="D27" s="143"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
@@ -2482,14 +2501,14 @@
       <c r="I27" s="15"/>
     </row>
     <row r="28" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A28" s="52"/>
-      <c r="B28" s="95" t="s">
+      <c r="A28" s="51"/>
+      <c r="B28" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="82" t="s">
+      <c r="C28" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="D28" s="144"/>
+      <c r="D28" s="143"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
@@ -2497,14 +2516,14 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A29" s="52"/>
-      <c r="B29" s="95" t="s">
+      <c r="A29" s="51"/>
+      <c r="B29" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="D29" s="144"/>
+      <c r="D29" s="143"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
@@ -2512,14 +2531,14 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" s="16" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A30" s="52"/>
-      <c r="B30" s="95" t="s">
+      <c r="A30" s="51"/>
+      <c r="B30" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="82" t="s">
+      <c r="C30" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="142"/>
+      <c r="D30" s="141"/>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
@@ -2527,14 +2546,14 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" s="16" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A31" s="52"/>
-      <c r="B31" s="95" t="s">
+      <c r="A31" s="51"/>
+      <c r="B31" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="82" t="s">
+      <c r="C31" s="81" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="144"/>
+      <c r="D31" s="143"/>
       <c r="E31" s="18"/>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
@@ -2542,14 +2561,14 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" s="16" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A32" s="52"/>
-      <c r="B32" s="70" t="s">
+      <c r="A32" s="51"/>
+      <c r="B32" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="82" t="s">
+      <c r="C32" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="145"/>
+      <c r="D32" s="144"/>
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
@@ -2557,14 +2576,14 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A33" s="52"/>
-      <c r="B33" s="70" t="s">
+      <c r="A33" s="51"/>
+      <c r="B33" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="82" t="s">
+      <c r="C33" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="146"/>
+      <c r="D33" s="145"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
       <c r="G33" s="20"/>
@@ -2572,29 +2591,29 @@
       <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" s="16" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A34" s="52"/>
-      <c r="B34" s="70" t="s">
+      <c r="A34" s="51"/>
+      <c r="B34" s="69" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="82" t="s">
+      <c r="C34" s="81" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="148"/>
+      <c r="D34" s="147"/>
       <c r="E34" s="21"/>
-      <c r="F34" s="101"/>
+      <c r="F34" s="100"/>
       <c r="G34" s="21"/>
       <c r="H34" s="21"/>
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="53"/>
-      <c r="B35" s="70" t="s">
+      <c r="A35" s="52"/>
+      <c r="B35" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="82" t="s">
+      <c r="C35" s="81" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="144"/>
+      <c r="D35" s="143"/>
       <c r="E35" s="18"/>
       <c r="F35" s="18"/>
       <c r="G35" s="18"/>
@@ -2602,14 +2621,14 @@
       <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:9" s="16" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A36" s="52"/>
-      <c r="B36" s="70" t="s">
+      <c r="A36" s="51"/>
+      <c r="B36" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="82" t="s">
+      <c r="C36" s="81" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="145"/>
+      <c r="D36" s="144"/>
       <c r="E36" s="19"/>
       <c r="F36" s="19"/>
       <c r="G36" s="19"/>
@@ -2617,14 +2636,14 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" s="16" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A37" s="52"/>
-      <c r="B37" s="70" t="s">
+      <c r="A37" s="51"/>
+      <c r="B37" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="82" t="s">
+      <c r="C37" s="81" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="145"/>
+      <c r="D37" s="144"/>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
@@ -2632,11 +2651,11 @@
       <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" s="25" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="91" t="s">
+      <c r="A38" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="63"/>
-      <c r="C38" s="83" t="s">
+      <c r="B38" s="62"/>
+      <c r="C38" s="82" t="s">
         <v>77</v>
       </c>
       <c r="D38" s="24"/>
@@ -2647,14 +2666,14 @@
       <c r="I38" s="24"/>
     </row>
     <row r="39" spans="1:9" s="28" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A39" s="54"/>
-      <c r="B39" s="71" t="s">
-        <v>205</v>
-      </c>
-      <c r="C39" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="D39" s="150"/>
+      <c r="A39" s="53"/>
+      <c r="B39" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="C39" s="83" t="s">
+        <v>203</v>
+      </c>
+      <c r="D39" s="149"/>
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
       <c r="G39" s="26"/>
@@ -2662,12 +2681,12 @@
       <c r="I39" s="27"/>
     </row>
     <row r="40" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="54"/>
-      <c r="B40" s="71" t="s">
-        <v>207</v>
-      </c>
-      <c r="C40" s="84"/>
-      <c r="D40" s="150"/>
+      <c r="A40" s="53"/>
+      <c r="B40" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="C40" s="83"/>
+      <c r="D40" s="149"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
@@ -2675,12 +2694,12 @@
       <c r="I40" s="27"/>
     </row>
     <row r="41" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="54"/>
-      <c r="B41" s="71" t="s">
-        <v>208</v>
-      </c>
-      <c r="C41" s="84"/>
-      <c r="D41" s="150"/>
+      <c r="A41" s="53"/>
+      <c r="B41" s="70" t="s">
+        <v>205</v>
+      </c>
+      <c r="C41" s="83"/>
+      <c r="D41" s="149"/>
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
       <c r="G41" s="26"/>
@@ -2688,12 +2707,12 @@
       <c r="I41" s="27"/>
     </row>
     <row r="42" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A42" s="54"/>
-      <c r="B42" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="C42" s="84"/>
-      <c r="D42" s="150"/>
+      <c r="A42" s="53"/>
+      <c r="B42" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="C42" s="83"/>
+      <c r="D42" s="149"/>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
@@ -2701,12 +2720,12 @@
       <c r="I42" s="27"/>
     </row>
     <row r="43" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A43" s="54"/>
-      <c r="B43" s="71" t="s">
-        <v>210</v>
-      </c>
-      <c r="C43" s="84"/>
-      <c r="D43" s="150"/>
+      <c r="A43" s="53"/>
+      <c r="B43" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="C43" s="83"/>
+      <c r="D43" s="149"/>
       <c r="E43" s="26"/>
       <c r="F43" s="26"/>
       <c r="G43" s="26"/>
@@ -2714,12 +2733,12 @@
       <c r="I43" s="27"/>
     </row>
     <row r="44" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A44" s="54"/>
-      <c r="B44" s="71" t="s">
-        <v>211</v>
-      </c>
-      <c r="C44" s="84"/>
-      <c r="D44" s="150"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="70" t="s">
+        <v>208</v>
+      </c>
+      <c r="C44" s="83"/>
+      <c r="D44" s="149"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
@@ -2727,581 +2746,644 @@
       <c r="I44" s="27"/>
     </row>
     <row r="45" spans="1:9" s="28" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A45" s="54"/>
-      <c r="B45" s="72" t="s">
+      <c r="A45" s="53"/>
+      <c r="B45" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="C45" s="83" t="s">
+        <v>215</v>
+      </c>
+      <c r="D45" s="159"/>
+      <c r="E45" s="160"/>
+      <c r="F45" s="161"/>
+      <c r="G45" s="160"/>
+      <c r="H45" s="160"/>
+      <c r="I45" s="27"/>
+    </row>
+    <row r="46" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A46" s="53"/>
+      <c r="B46" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="C46" s="83"/>
+      <c r="D46" s="159"/>
+      <c r="E46" s="160"/>
+      <c r="F46" s="161"/>
+      <c r="G46" s="160"/>
+      <c r="H46" s="160"/>
+      <c r="I46" s="27"/>
+    </row>
+    <row r="47" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A47" s="53"/>
+      <c r="B47" s="71" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="83"/>
+      <c r="D47" s="159"/>
+      <c r="E47" s="160"/>
+      <c r="F47" s="161"/>
+      <c r="G47" s="160"/>
+      <c r="H47" s="160"/>
+      <c r="I47" s="27"/>
+    </row>
+    <row r="48" spans="1:9" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A48" s="53"/>
+      <c r="B48" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" s="83"/>
+      <c r="D48" s="159"/>
+      <c r="E48" s="160"/>
+      <c r="F48" s="161"/>
+      <c r="G48" s="160"/>
+      <c r="H48" s="160"/>
+      <c r="I48" s="27"/>
+    </row>
+    <row r="49" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A49" s="53"/>
+      <c r="B49" s="71" t="s">
+        <v>213</v>
+      </c>
+      <c r="C49" s="83"/>
+      <c r="D49" s="159"/>
+      <c r="E49" s="160"/>
+      <c r="F49" s="161"/>
+      <c r="G49" s="160"/>
+      <c r="H49" s="160"/>
+      <c r="I49" s="27"/>
+    </row>
+    <row r="50" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A50" s="53"/>
+      <c r="B50" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="C50" s="83"/>
+      <c r="D50" s="159"/>
+      <c r="E50" s="160"/>
+      <c r="F50" s="161"/>
+      <c r="G50" s="160"/>
+      <c r="H50" s="160"/>
+      <c r="I50" s="27"/>
+    </row>
+    <row r="51" spans="1:47" s="28" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A51" s="53"/>
+      <c r="B51" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C45" s="84" t="s">
-        <v>79</v>
-      </c>
-      <c r="D45" s="150"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
-      <c r="I45" s="27"/>
-    </row>
-    <row r="46" spans="1:9" s="28" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A46" s="54"/>
-      <c r="B46" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="84" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="150"/>
-      <c r="E46" s="150"/>
-      <c r="F46" s="150"/>
-      <c r="G46" s="150"/>
-      <c r="H46" s="150"/>
-      <c r="I46" s="27"/>
-    </row>
-    <row r="47" spans="1:9" s="28" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A47" s="54"/>
-      <c r="B47" s="92" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="84" t="s">
-        <v>84</v>
-      </c>
-      <c r="D47" s="150"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="27"/>
-    </row>
-    <row r="48" spans="1:9" s="32" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A48" s="98" t="s">
-        <v>85</v>
-      </c>
-      <c r="B48" s="64"/>
-      <c r="C48" s="85" t="s">
-        <v>86</v>
-      </c>
-      <c r="D48" s="151"/>
-      <c r="E48" s="30"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
-      <c r="I48" s="31"/>
-    </row>
-    <row r="49" spans="1:47" s="35" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A49" s="55"/>
-      <c r="B49" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="86" t="s">
-        <v>88</v>
-      </c>
-      <c r="D49" s="152"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="34"/>
-    </row>
-    <row r="50" spans="1:47" s="35" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
-      <c r="A50" s="55"/>
-      <c r="B50" s="73" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" s="86" t="s">
-        <v>90</v>
-      </c>
-      <c r="D50" s="153"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="34"/>
-    </row>
-    <row r="51" spans="1:47" s="35" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A51" s="55"/>
-      <c r="B51" s="73" t="s">
-        <v>91</v>
-      </c>
-      <c r="C51" s="86" t="s">
-        <v>92</v>
-      </c>
-      <c r="D51" s="154"/>
+      <c r="C51" s="83"/>
+      <c r="D51" s="149"/>
       <c r="E51" s="149"/>
       <c r="F51" s="149"/>
       <c r="G51" s="149"/>
       <c r="H51" s="149"/>
-      <c r="I51" s="34"/>
-    </row>
-    <row r="52" spans="1:47" s="35" customFormat="1" ht="57" x14ac:dyDescent="0.5">
-      <c r="A52" s="55"/>
-      <c r="B52" s="73" t="s">
+      <c r="I51" s="27"/>
+    </row>
+    <row r="52" spans="1:47" s="28" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A52" s="53"/>
+      <c r="B52" s="91" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" s="83" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="149"/>
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="I52" s="27"/>
+    </row>
+    <row r="53" spans="1:47" s="31" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A53" s="97" t="s">
+        <v>82</v>
+      </c>
+      <c r="B53" s="63"/>
+      <c r="C53" s="84" t="s">
+        <v>83</v>
+      </c>
+      <c r="D53" s="150"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="30"/>
+    </row>
+    <row r="54" spans="1:47" s="34" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A54" s="54"/>
+      <c r="B54" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" s="85" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="151"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
+      <c r="H54" s="32"/>
+      <c r="I54" s="33"/>
+    </row>
+    <row r="55" spans="1:47" s="34" customFormat="1" ht="79.8" x14ac:dyDescent="0.5">
+      <c r="A55" s="54"/>
+      <c r="B55" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="85" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="152"/>
+      <c r="E55" s="35"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="35"/>
+      <c r="I55" s="33"/>
+    </row>
+    <row r="56" spans="1:47" s="34" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A56" s="54"/>
+      <c r="B56" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="85" t="s">
+        <v>89</v>
+      </c>
+      <c r="D56" s="153"/>
+      <c r="E56" s="148"/>
+      <c r="F56" s="148"/>
+      <c r="G56" s="148"/>
+      <c r="H56" s="148"/>
+      <c r="I56" s="33"/>
+    </row>
+    <row r="57" spans="1:47" s="34" customFormat="1" ht="57" x14ac:dyDescent="0.5">
+      <c r="A57" s="54"/>
+      <c r="B57" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="C57" s="85" t="s">
+        <v>92</v>
+      </c>
+      <c r="D57" s="154"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="33"/>
+    </row>
+    <row r="58" spans="1:47" s="34" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
+      <c r="A58" s="54"/>
+      <c r="B58" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="C52" s="86" t="s">
+      <c r="D58" s="152"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
+      <c r="H58" s="35"/>
+      <c r="I58" s="33"/>
+    </row>
+    <row r="59" spans="1:47" s="34" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A59" s="54"/>
+      <c r="B59" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="D52" s="155"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="34"/>
-    </row>
-    <row r="53" spans="1:47" s="35" customFormat="1" ht="91.2" x14ac:dyDescent="0.5">
-      <c r="A53" s="55"/>
-      <c r="B53" s="73" t="s">
+      <c r="C59" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="C53" s="86" t="s">
-        <v>97</v>
-      </c>
-      <c r="D53" s="153"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="34"/>
-    </row>
-    <row r="54" spans="1:47" s="35" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A54" s="55"/>
-      <c r="B54" s="73" t="s">
+      <c r="D59" s="148"/>
+      <c r="E59" s="148"/>
+      <c r="F59" s="148"/>
+      <c r="G59" s="148"/>
+      <c r="H59" s="148"/>
+      <c r="I59" s="33"/>
+    </row>
+    <row r="60" spans="1:47" s="38" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A60" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="C54" s="86" t="s">
+      <c r="B60" s="64"/>
+      <c r="C60" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="D54" s="149"/>
-      <c r="E54" s="149"/>
-      <c r="F54" s="149"/>
-      <c r="G54" s="149"/>
-      <c r="H54" s="149"/>
-      <c r="I54" s="34"/>
-    </row>
-    <row r="55" spans="1:47" s="39" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A55" s="56" t="s">
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+    </row>
+    <row r="61" spans="1:47" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A61" s="56"/>
+      <c r="B61" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="65"/>
-      <c r="C55" s="87" t="s">
+      <c r="D61" s="155"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="39"/>
+      <c r="H61" s="39"/>
+      <c r="I61" s="40"/>
+    </row>
+    <row r="62" spans="1:47" s="41" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A62" s="56"/>
+      <c r="B62" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="D55" s="38"/>
-      <c r="E55" s="38"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="38"/>
-      <c r="H55" s="38"/>
-      <c r="I55" s="38"/>
-    </row>
-    <row r="56" spans="1:47" s="42" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="57"/>
-      <c r="B56" s="74" t="s">
+      <c r="C62" s="87" t="s">
         <v>103</v>
       </c>
-      <c r="C56" s="88" t="s">
+      <c r="D62" s="155"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
+      <c r="I62" s="40"/>
+    </row>
+    <row r="63" spans="1:47" s="41" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A63" s="56"/>
+      <c r="B63" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="D56" s="156"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="41"/>
-    </row>
-    <row r="57" spans="1:47" s="42" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A57" s="57"/>
-      <c r="B57" s="74" t="s">
+      <c r="C63" s="87" t="s">
         <v>105</v>
       </c>
-      <c r="C57" s="88" t="s">
+      <c r="D63" s="155"/>
+      <c r="E63" s="155"/>
+      <c r="F63" s="155"/>
+      <c r="G63" s="155"/>
+      <c r="H63" s="155"/>
+      <c r="I63" s="56"/>
+    </row>
+    <row r="64" spans="1:47" s="42" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A64" s="56"/>
+      <c r="B64" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="156"/>
-      <c r="E57" s="40"/>
-      <c r="F57" s="40"/>
-      <c r="G57" s="40"/>
-      <c r="H57" s="40"/>
-      <c r="I57" s="41"/>
-    </row>
-    <row r="58" spans="1:47" s="42" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="57"/>
-      <c r="B58" s="74" t="s">
+      <c r="C64" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="C58" s="88" t="s">
+      <c r="D64" s="155"/>
+      <c r="E64" s="155"/>
+      <c r="F64" s="155"/>
+      <c r="G64" s="155"/>
+      <c r="H64" s="155"/>
+      <c r="I64" s="56"/>
+      <c r="J64" s="56"/>
+      <c r="K64" s="56"/>
+      <c r="L64" s="56"/>
+      <c r="M64" s="56"/>
+      <c r="N64" s="56"/>
+      <c r="O64" s="56"/>
+      <c r="P64" s="56"/>
+      <c r="Q64" s="56"/>
+      <c r="R64" s="56"/>
+      <c r="S64" s="56"/>
+      <c r="T64" s="56"/>
+      <c r="U64" s="56"/>
+      <c r="V64" s="56"/>
+      <c r="W64" s="56"/>
+      <c r="X64" s="56"/>
+      <c r="Y64" s="56"/>
+      <c r="Z64" s="56"/>
+      <c r="AA64" s="56"/>
+      <c r="AB64" s="56"/>
+      <c r="AC64" s="56"/>
+      <c r="AD64" s="56"/>
+      <c r="AE64" s="56"/>
+      <c r="AF64" s="56"/>
+      <c r="AG64" s="56"/>
+      <c r="AH64" s="56"/>
+      <c r="AI64" s="56"/>
+      <c r="AJ64" s="56"/>
+      <c r="AK64" s="56"/>
+      <c r="AL64" s="56"/>
+      <c r="AM64" s="56"/>
+      <c r="AN64" s="56"/>
+      <c r="AO64" s="56"/>
+      <c r="AP64" s="56"/>
+      <c r="AQ64" s="56"/>
+      <c r="AR64" s="56"/>
+      <c r="AS64" s="56"/>
+      <c r="AT64" s="56"/>
+      <c r="AU64" s="56"/>
+    </row>
+    <row r="65" spans="1:47" s="45" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A65" s="56"/>
+      <c r="B65" s="73" t="s">
         <v>108</v>
       </c>
-      <c r="D58" s="156"/>
-      <c r="E58" s="156"/>
-      <c r="F58" s="156"/>
-      <c r="G58" s="156"/>
-      <c r="H58" s="156"/>
-      <c r="I58" s="57"/>
-    </row>
-    <row r="59" spans="1:47" s="43" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A59" s="57"/>
-      <c r="B59" s="74" t="s">
+      <c r="C65" s="87"/>
+      <c r="D65" s="155"/>
+      <c r="E65" s="155"/>
+      <c r="F65" s="155"/>
+      <c r="G65" s="155"/>
+      <c r="H65" s="155"/>
+      <c r="I65" s="56"/>
+      <c r="J65" s="56"/>
+      <c r="K65" s="56"/>
+      <c r="L65" s="56"/>
+      <c r="M65" s="56"/>
+      <c r="N65" s="56"/>
+      <c r="O65" s="56"/>
+      <c r="P65" s="56"/>
+      <c r="Q65" s="56"/>
+      <c r="R65" s="56"/>
+      <c r="S65" s="56"/>
+      <c r="T65" s="56"/>
+      <c r="U65" s="56"/>
+      <c r="V65" s="56"/>
+      <c r="W65" s="56"/>
+      <c r="X65" s="56"/>
+      <c r="Y65" s="56"/>
+      <c r="Z65" s="56"/>
+      <c r="AA65" s="56"/>
+      <c r="AB65" s="56"/>
+      <c r="AC65" s="56"/>
+      <c r="AD65" s="56"/>
+      <c r="AE65" s="56"/>
+      <c r="AF65" s="56"/>
+      <c r="AG65" s="56"/>
+      <c r="AH65" s="56"/>
+      <c r="AI65" s="56"/>
+      <c r="AJ65" s="56"/>
+      <c r="AK65" s="56"/>
+      <c r="AL65" s="56"/>
+      <c r="AM65" s="56"/>
+      <c r="AN65" s="56"/>
+      <c r="AO65" s="56"/>
+      <c r="AP65" s="56"/>
+      <c r="AQ65" s="56"/>
+      <c r="AR65" s="56"/>
+      <c r="AS65" s="56"/>
+      <c r="AT65" s="56"/>
+      <c r="AU65" s="56"/>
+    </row>
+    <row r="66" spans="1:47" s="45" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A66" s="56"/>
+      <c r="B66" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="C59" s="88" t="s">
+      <c r="C66" s="87"/>
+      <c r="D66" s="155"/>
+      <c r="E66" s="155"/>
+      <c r="F66" s="155"/>
+      <c r="G66" s="155"/>
+      <c r="H66" s="155"/>
+      <c r="I66" s="56"/>
+      <c r="J66" s="56"/>
+      <c r="K66" s="56"/>
+      <c r="L66" s="56"/>
+      <c r="M66" s="56"/>
+      <c r="N66" s="56"/>
+      <c r="O66" s="56"/>
+      <c r="P66" s="56"/>
+      <c r="Q66" s="56"/>
+      <c r="R66" s="56"/>
+      <c r="S66" s="56"/>
+      <c r="T66" s="56"/>
+      <c r="U66" s="56"/>
+      <c r="V66" s="56"/>
+      <c r="W66" s="56"/>
+      <c r="X66" s="56"/>
+      <c r="Y66" s="56"/>
+      <c r="Z66" s="56"/>
+      <c r="AA66" s="56"/>
+      <c r="AB66" s="56"/>
+      <c r="AC66" s="56"/>
+      <c r="AD66" s="56"/>
+      <c r="AE66" s="56"/>
+      <c r="AF66" s="56"/>
+      <c r="AG66" s="56"/>
+      <c r="AH66" s="56"/>
+      <c r="AI66" s="56"/>
+      <c r="AJ66" s="56"/>
+      <c r="AK66" s="56"/>
+      <c r="AL66" s="56"/>
+      <c r="AM66" s="56"/>
+      <c r="AN66" s="56"/>
+      <c r="AO66" s="56"/>
+      <c r="AP66" s="56"/>
+      <c r="AQ66" s="56"/>
+      <c r="AR66" s="56"/>
+      <c r="AS66" s="56"/>
+      <c r="AT66" s="56"/>
+      <c r="AU66" s="56"/>
+    </row>
+    <row r="67" spans="1:47" s="45" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A67" s="56"/>
+      <c r="B67" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="D59" s="156"/>
-      <c r="E59" s="156"/>
-      <c r="F59" s="156"/>
-      <c r="G59" s="156"/>
-      <c r="H59" s="156"/>
-      <c r="I59" s="57"/>
-      <c r="J59" s="57"/>
-      <c r="K59" s="57"/>
-      <c r="L59" s="57"/>
-      <c r="M59" s="57"/>
-      <c r="N59" s="57"/>
-      <c r="O59" s="57"/>
-      <c r="P59" s="57"/>
-      <c r="Q59" s="57"/>
-      <c r="R59" s="57"/>
-      <c r="S59" s="57"/>
-      <c r="T59" s="57"/>
-      <c r="U59" s="57"/>
-      <c r="V59" s="57"/>
-      <c r="W59" s="57"/>
-      <c r="X59" s="57"/>
-      <c r="Y59" s="57"/>
-      <c r="Z59" s="57"/>
-      <c r="AA59" s="57"/>
-      <c r="AB59" s="57"/>
-      <c r="AC59" s="57"/>
-      <c r="AD59" s="57"/>
-      <c r="AE59" s="57"/>
-      <c r="AF59" s="57"/>
-      <c r="AG59" s="57"/>
-      <c r="AH59" s="57"/>
-      <c r="AI59" s="57"/>
-      <c r="AJ59" s="57"/>
-      <c r="AK59" s="57"/>
-      <c r="AL59" s="57"/>
-      <c r="AM59" s="57"/>
-      <c r="AN59" s="57"/>
-      <c r="AO59" s="57"/>
-      <c r="AP59" s="57"/>
-      <c r="AQ59" s="57"/>
-      <c r="AR59" s="57"/>
-      <c r="AS59" s="57"/>
-      <c r="AT59" s="57"/>
-      <c r="AU59" s="57"/>
-    </row>
-    <row r="60" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="57"/>
-      <c r="B60" s="74" t="s">
+      <c r="C67" s="87"/>
+      <c r="D67" s="155"/>
+      <c r="E67" s="155"/>
+      <c r="F67" s="155"/>
+      <c r="G67" s="155"/>
+      <c r="H67" s="155"/>
+      <c r="I67" s="56"/>
+      <c r="J67" s="56"/>
+      <c r="K67" s="56"/>
+      <c r="L67" s="56"/>
+      <c r="M67" s="56"/>
+      <c r="N67" s="56"/>
+      <c r="O67" s="56"/>
+      <c r="P67" s="56"/>
+      <c r="Q67" s="56"/>
+      <c r="R67" s="56"/>
+      <c r="S67" s="56"/>
+      <c r="T67" s="56"/>
+      <c r="U67" s="56"/>
+      <c r="V67" s="56"/>
+      <c r="W67" s="56"/>
+      <c r="X67" s="56"/>
+      <c r="Y67" s="56"/>
+      <c r="Z67" s="56"/>
+      <c r="AA67" s="56"/>
+      <c r="AB67" s="56"/>
+      <c r="AC67" s="56"/>
+      <c r="AD67" s="56"/>
+      <c r="AE67" s="56"/>
+      <c r="AF67" s="56"/>
+      <c r="AG67" s="56"/>
+      <c r="AH67" s="56"/>
+      <c r="AI67" s="56"/>
+      <c r="AJ67" s="56"/>
+      <c r="AK67" s="56"/>
+      <c r="AL67" s="56"/>
+      <c r="AM67" s="56"/>
+      <c r="AN67" s="56"/>
+      <c r="AO67" s="56"/>
+      <c r="AP67" s="56"/>
+      <c r="AQ67" s="56"/>
+      <c r="AR67" s="56"/>
+      <c r="AS67" s="56"/>
+      <c r="AT67" s="56"/>
+      <c r="AU67" s="56"/>
+    </row>
+    <row r="68" spans="1:47" s="45" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A68" s="56"/>
+      <c r="B68" s="73" t="s">
         <v>111</v>
       </c>
-      <c r="C60" s="88"/>
-      <c r="D60" s="156"/>
-      <c r="E60" s="156"/>
-      <c r="F60" s="156"/>
-      <c r="G60" s="156"/>
-      <c r="H60" s="156"/>
-      <c r="I60" s="57"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
-      <c r="L60" s="57"/>
-      <c r="M60" s="57"/>
-      <c r="N60" s="57"/>
-      <c r="O60" s="57"/>
-      <c r="P60" s="57"/>
-      <c r="Q60" s="57"/>
-      <c r="R60" s="57"/>
-      <c r="S60" s="57"/>
-      <c r="T60" s="57"/>
-      <c r="U60" s="57"/>
-      <c r="V60" s="57"/>
-      <c r="W60" s="57"/>
-      <c r="X60" s="57"/>
-      <c r="Y60" s="57"/>
-      <c r="Z60" s="57"/>
-      <c r="AA60" s="57"/>
-      <c r="AB60" s="57"/>
-      <c r="AC60" s="57"/>
-      <c r="AD60" s="57"/>
-      <c r="AE60" s="57"/>
-      <c r="AF60" s="57"/>
-      <c r="AG60" s="57"/>
-      <c r="AH60" s="57"/>
-      <c r="AI60" s="57"/>
-      <c r="AJ60" s="57"/>
-      <c r="AK60" s="57"/>
-      <c r="AL60" s="57"/>
-      <c r="AM60" s="57"/>
-      <c r="AN60" s="57"/>
-      <c r="AO60" s="57"/>
-      <c r="AP60" s="57"/>
-      <c r="AQ60" s="57"/>
-      <c r="AR60" s="57"/>
-      <c r="AS60" s="57"/>
-      <c r="AT60" s="57"/>
-      <c r="AU60" s="57"/>
-    </row>
-    <row r="61" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="57"/>
-      <c r="B61" s="74" t="s">
+      <c r="C68" s="87"/>
+      <c r="D68" s="155"/>
+      <c r="E68" s="155"/>
+      <c r="F68" s="155"/>
+      <c r="G68" s="155"/>
+      <c r="H68" s="155"/>
+      <c r="I68" s="56"/>
+      <c r="J68" s="56"/>
+      <c r="K68" s="56"/>
+      <c r="L68" s="56"/>
+      <c r="M68" s="56"/>
+      <c r="N68" s="56"/>
+      <c r="O68" s="56"/>
+      <c r="P68" s="56"/>
+      <c r="Q68" s="56"/>
+      <c r="R68" s="56"/>
+      <c r="S68" s="56"/>
+      <c r="T68" s="56"/>
+      <c r="U68" s="56"/>
+      <c r="V68" s="56"/>
+      <c r="W68" s="56"/>
+      <c r="X68" s="56"/>
+      <c r="Y68" s="56"/>
+      <c r="Z68" s="56"/>
+      <c r="AA68" s="56"/>
+      <c r="AB68" s="56"/>
+      <c r="AC68" s="56"/>
+      <c r="AD68" s="56"/>
+      <c r="AE68" s="56"/>
+      <c r="AF68" s="56"/>
+      <c r="AG68" s="56"/>
+      <c r="AH68" s="56"/>
+      <c r="AI68" s="56"/>
+      <c r="AJ68" s="56"/>
+      <c r="AK68" s="56"/>
+      <c r="AL68" s="56"/>
+      <c r="AM68" s="56"/>
+      <c r="AN68" s="56"/>
+      <c r="AO68" s="56"/>
+      <c r="AP68" s="56"/>
+      <c r="AQ68" s="56"/>
+      <c r="AR68" s="56"/>
+      <c r="AS68" s="56"/>
+      <c r="AT68" s="56"/>
+      <c r="AU68" s="56"/>
+    </row>
+    <row r="69" spans="1:47" s="105" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A69" s="101" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="102"/>
+      <c r="C69" s="103"/>
+      <c r="D69" s="104"/>
+      <c r="E69" s="104"/>
+      <c r="F69" s="104"/>
+      <c r="G69" s="104"/>
+      <c r="H69" s="104"/>
+      <c r="I69" s="104"/>
+    </row>
+    <row r="70" spans="1:47" s="45" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A70" s="57"/>
+      <c r="B70" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="C61" s="88"/>
-      <c r="D61" s="156"/>
-      <c r="E61" s="156"/>
-      <c r="F61" s="156"/>
-      <c r="G61" s="156"/>
-      <c r="H61" s="156"/>
-      <c r="I61" s="57"/>
-      <c r="J61" s="57"/>
-      <c r="K61" s="57"/>
-      <c r="L61" s="57"/>
-      <c r="M61" s="57"/>
-      <c r="N61" s="57"/>
-      <c r="O61" s="57"/>
-      <c r="P61" s="57"/>
-      <c r="Q61" s="57"/>
-      <c r="R61" s="57"/>
-      <c r="S61" s="57"/>
-      <c r="T61" s="57"/>
-      <c r="U61" s="57"/>
-      <c r="V61" s="57"/>
-      <c r="W61" s="57"/>
-      <c r="X61" s="57"/>
-      <c r="Y61" s="57"/>
-      <c r="Z61" s="57"/>
-      <c r="AA61" s="57"/>
-      <c r="AB61" s="57"/>
-      <c r="AC61" s="57"/>
-      <c r="AD61" s="57"/>
-      <c r="AE61" s="57"/>
-      <c r="AF61" s="57"/>
-      <c r="AG61" s="57"/>
-      <c r="AH61" s="57"/>
-      <c r="AI61" s="57"/>
-      <c r="AJ61" s="57"/>
-      <c r="AK61" s="57"/>
-      <c r="AL61" s="57"/>
-      <c r="AM61" s="57"/>
-      <c r="AN61" s="57"/>
-      <c r="AO61" s="57"/>
-      <c r="AP61" s="57"/>
-      <c r="AQ61" s="57"/>
-      <c r="AR61" s="57"/>
-      <c r="AS61" s="57"/>
-      <c r="AT61" s="57"/>
-      <c r="AU61" s="57"/>
-    </row>
-    <row r="62" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="57"/>
-      <c r="B62" s="74" t="s">
+      <c r="C70" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="C62" s="88"/>
-      <c r="D62" s="156"/>
-      <c r="E62" s="156"/>
-      <c r="F62" s="156"/>
-      <c r="G62" s="156"/>
-      <c r="H62" s="156"/>
-      <c r="I62" s="57"/>
-      <c r="J62" s="57"/>
-      <c r="K62" s="57"/>
-      <c r="L62" s="57"/>
-      <c r="M62" s="57"/>
-      <c r="N62" s="57"/>
-      <c r="O62" s="57"/>
-      <c r="P62" s="57"/>
-      <c r="Q62" s="57"/>
-      <c r="R62" s="57"/>
-      <c r="S62" s="57"/>
-      <c r="T62" s="57"/>
-      <c r="U62" s="57"/>
-      <c r="V62" s="57"/>
-      <c r="W62" s="57"/>
-      <c r="X62" s="57"/>
-      <c r="Y62" s="57"/>
-      <c r="Z62" s="57"/>
-      <c r="AA62" s="57"/>
-      <c r="AB62" s="57"/>
-      <c r="AC62" s="57"/>
-      <c r="AD62" s="57"/>
-      <c r="AE62" s="57"/>
-      <c r="AF62" s="57"/>
-      <c r="AG62" s="57"/>
-      <c r="AH62" s="57"/>
-      <c r="AI62" s="57"/>
-      <c r="AJ62" s="57"/>
-      <c r="AK62" s="57"/>
-      <c r="AL62" s="57"/>
-      <c r="AM62" s="57"/>
-      <c r="AN62" s="57"/>
-      <c r="AO62" s="57"/>
-      <c r="AP62" s="57"/>
-      <c r="AQ62" s="57"/>
-      <c r="AR62" s="57"/>
-      <c r="AS62" s="57"/>
-      <c r="AT62" s="57"/>
-      <c r="AU62" s="57"/>
-    </row>
-    <row r="63" spans="1:47" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="57"/>
-      <c r="B63" s="74" t="s">
+      <c r="D70" s="156"/>
+      <c r="E70" s="156"/>
+      <c r="F70" s="156"/>
+      <c r="G70" s="156"/>
+      <c r="H70" s="43"/>
+      <c r="I70" s="44"/>
+    </row>
+    <row r="71" spans="1:47" s="45" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A71" s="57"/>
+      <c r="B71" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="C63" s="88"/>
-      <c r="D63" s="156"/>
-      <c r="E63" s="156"/>
-      <c r="F63" s="156"/>
-      <c r="G63" s="156"/>
-      <c r="H63" s="156"/>
-      <c r="I63" s="57"/>
-      <c r="J63" s="57"/>
-      <c r="K63" s="57"/>
-      <c r="L63" s="57"/>
-      <c r="M63" s="57"/>
-      <c r="N63" s="57"/>
-      <c r="O63" s="57"/>
-      <c r="P63" s="57"/>
-      <c r="Q63" s="57"/>
-      <c r="R63" s="57"/>
-      <c r="S63" s="57"/>
-      <c r="T63" s="57"/>
-      <c r="U63" s="57"/>
-      <c r="V63" s="57"/>
-      <c r="W63" s="57"/>
-      <c r="X63" s="57"/>
-      <c r="Y63" s="57"/>
-      <c r="Z63" s="57"/>
-      <c r="AA63" s="57"/>
-      <c r="AB63" s="57"/>
-      <c r="AC63" s="57"/>
-      <c r="AD63" s="57"/>
-      <c r="AE63" s="57"/>
-      <c r="AF63" s="57"/>
-      <c r="AG63" s="57"/>
-      <c r="AH63" s="57"/>
-      <c r="AI63" s="57"/>
-      <c r="AJ63" s="57"/>
-      <c r="AK63" s="57"/>
-      <c r="AL63" s="57"/>
-      <c r="AM63" s="57"/>
-      <c r="AN63" s="57"/>
-      <c r="AO63" s="57"/>
-      <c r="AP63" s="57"/>
-      <c r="AQ63" s="57"/>
-      <c r="AR63" s="57"/>
-      <c r="AS63" s="57"/>
-      <c r="AT63" s="57"/>
-      <c r="AU63" s="57"/>
-    </row>
-    <row r="64" spans="1:47" s="106" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A64" s="102" t="s">
-        <v>168</v>
-      </c>
-      <c r="B64" s="103"/>
-      <c r="C64" s="104"/>
-      <c r="D64" s="105"/>
-      <c r="E64" s="105"/>
-      <c r="F64" s="105"/>
-      <c r="G64" s="105"/>
-      <c r="H64" s="105"/>
-      <c r="I64" s="105"/>
-    </row>
-    <row r="65" spans="1:9" s="46" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A65" s="58"/>
-      <c r="B65" s="75" t="s">
+      <c r="C71" s="88"/>
+      <c r="D71" s="156"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="43"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="44"/>
+    </row>
+    <row r="72" spans="1:47" s="45" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A72" s="57"/>
+      <c r="B72" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="C65" s="89" t="s">
+      <c r="C72" s="88"/>
+      <c r="D72" s="156"/>
+      <c r="E72" s="43"/>
+      <c r="F72" s="43"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="44"/>
+    </row>
+    <row r="73" spans="1:47" s="45" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+      <c r="A73" s="57"/>
+      <c r="B73" s="75" t="s">
         <v>116</v>
       </c>
-      <c r="D65" s="157"/>
-      <c r="E65" s="157"/>
-      <c r="F65" s="157"/>
-      <c r="G65" s="157"/>
-      <c r="H65" s="44"/>
-      <c r="I65" s="45"/>
-    </row>
-    <row r="66" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="58"/>
-      <c r="B66" s="75" t="s">
+      <c r="C73" s="88"/>
+      <c r="D73" s="156"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="43"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="43"/>
+      <c r="I73" s="44"/>
+    </row>
+    <row r="74" spans="1:47" s="45" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
+      <c r="A74" s="57"/>
+      <c r="B74" s="75" t="s">
         <v>117</v>
       </c>
-      <c r="C66" s="89"/>
-      <c r="D66" s="157"/>
-      <c r="E66" s="44"/>
-      <c r="F66" s="44"/>
-      <c r="G66" s="44"/>
-      <c r="H66" s="44"/>
-      <c r="I66" s="45"/>
-    </row>
-    <row r="67" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A67" s="58"/>
-      <c r="B67" s="75" t="s">
+      <c r="C74" s="88"/>
+      <c r="D74" s="156"/>
+      <c r="E74" s="43"/>
+      <c r="F74" s="43"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="43"/>
+      <c r="I74" s="44"/>
+    </row>
+    <row r="75" spans="1:47" s="45" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A75" s="57"/>
+      <c r="B75" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="C67" s="89"/>
-      <c r="D67" s="157"/>
-      <c r="E67" s="44"/>
-      <c r="F67" s="44"/>
-      <c r="G67" s="44"/>
-      <c r="H67" s="44"/>
-      <c r="I67" s="45"/>
-    </row>
-    <row r="68" spans="1:9" s="46" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A68" s="58"/>
-      <c r="B68" s="76" t="s">
+      <c r="C75" s="88" t="s">
         <v>119</v>
       </c>
-      <c r="C68" s="89"/>
-      <c r="D68" s="157"/>
-      <c r="E68" s="44"/>
-      <c r="F68" s="44"/>
-      <c r="G68" s="44"/>
-      <c r="H68" s="44"/>
-      <c r="I68" s="45"/>
-    </row>
-    <row r="69" spans="1:9" s="46" customFormat="1" ht="26.4" x14ac:dyDescent="0.5">
-      <c r="A69" s="58"/>
-      <c r="B69" s="76" t="s">
+      <c r="D75" s="156"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="44"/>
+    </row>
+    <row r="76" spans="1:47" s="45" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A76" s="57"/>
+      <c r="B76" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="C69" s="89"/>
-      <c r="D69" s="157"/>
-      <c r="E69" s="44"/>
-      <c r="F69" s="44"/>
-      <c r="G69" s="44"/>
-      <c r="H69" s="44"/>
-      <c r="I69" s="45"/>
-    </row>
-    <row r="70" spans="1:9" s="46" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A70" s="58"/>
-      <c r="B70" s="75" t="s">
+      <c r="C76" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="C70" s="89" t="s">
-        <v>122</v>
-      </c>
-      <c r="D70" s="157"/>
-      <c r="E70" s="44"/>
-      <c r="F70" s="44"/>
-      <c r="G70" s="44"/>
-      <c r="H70" s="44"/>
-      <c r="I70" s="45"/>
-    </row>
-    <row r="71" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A71" s="58"/>
-      <c r="B71" s="75" t="s">
-        <v>123</v>
-      </c>
-      <c r="C71" s="89" t="s">
-        <v>124</v>
-      </c>
-      <c r="D71" s="157"/>
-      <c r="E71" s="44"/>
-      <c r="F71" s="44"/>
-      <c r="G71" s="44"/>
-      <c r="H71" s="44"/>
-      <c r="I71" s="45"/>
+      <c r="D76" s="156"/>
+      <c r="E76" s="43"/>
+      <c r="F76" s="43"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="43"/>
+      <c r="I76" s="44"/>
     </row>
   </sheetData>
   <sheetProtection deleteColumns="0" selectLockedCells="1"/>
@@ -3320,22 +3402,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" style="47" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="59" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="66" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="46" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" style="65" customWidth="1"/>
     <col min="4" max="8" width="32.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.5">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="65" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -3358,239 +3440,239 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="57" x14ac:dyDescent="0.5">
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="65" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="114" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
+      <c r="A3" s="112" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" s="115"/>
+      <c r="C3" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
+      <c r="G3" s="113"/>
+      <c r="H3" s="113"/>
+      <c r="I3" s="113"/>
+    </row>
+    <row r="4" spans="1:9" s="108" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.5">
+      <c r="A4" s="107"/>
+      <c r="B4" s="109" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="110" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="106"/>
+    </row>
+    <row r="5" spans="1:9" s="108" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
+      <c r="A5" s="107"/>
+      <c r="B5" s="109" t="s">
+        <v>168</v>
+      </c>
+      <c r="C5" s="110" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
+      <c r="G5" s="111"/>
+      <c r="H5" s="111"/>
+      <c r="I5" s="106"/>
+    </row>
+    <row r="6" spans="1:9" s="108" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A6" s="107"/>
+      <c r="B6" s="109" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="110" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="106"/>
+    </row>
+    <row r="7" spans="1:9" s="108" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A7" s="107"/>
+      <c r="B7" s="109" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="111"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="111"/>
+      <c r="G7" s="111"/>
+      <c r="H7" s="111"/>
+      <c r="I7" s="106"/>
+    </row>
+    <row r="8" spans="1:9" s="108" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
+      <c r="A8" s="107"/>
+      <c r="B8" s="109" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="115" customFormat="1" ht="34.200000000000003" x14ac:dyDescent="0.5">
-      <c r="A3" s="113" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="116"/>
-      <c r="C3" s="117" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-    </row>
-    <row r="4" spans="1:9" s="109" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.5">
-      <c r="A4" s="108"/>
-      <c r="B4" s="110" t="s">
-        <v>190</v>
-      </c>
-      <c r="C4" s="111" t="s">
-        <v>191</v>
-      </c>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
-      <c r="F4" s="112"/>
-      <c r="G4" s="112"/>
-      <c r="H4" s="112"/>
-      <c r="I4" s="107"/>
-    </row>
-    <row r="5" spans="1:9" s="109" customFormat="1" ht="68.400000000000006" x14ac:dyDescent="0.5">
-      <c r="A5" s="108"/>
-      <c r="B5" s="110" t="s">
+      <c r="C8" s="110" t="s">
         <v>171</v>
       </c>
-      <c r="C5" s="111" t="s">
+      <c r="D8" s="134"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="111"/>
+      <c r="G8" s="111"/>
+      <c r="H8" s="111"/>
+      <c r="I8" s="106"/>
+    </row>
+    <row r="9" spans="1:9" s="129" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A9" s="125" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" s="126"/>
+      <c r="C9" s="127" t="s">
+        <v>174</v>
+      </c>
+      <c r="D9" s="128"/>
+      <c r="E9" s="128"/>
+      <c r="F9" s="128"/>
+      <c r="G9" s="128"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="128"/>
+    </row>
+    <row r="10" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="117"/>
+      <c r="B10" s="121" t="s">
         <v>173</v>
       </c>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
-      <c r="F5" s="112"/>
-      <c r="G5" s="112"/>
-      <c r="H5" s="112"/>
-      <c r="I5" s="107"/>
-    </row>
-    <row r="6" spans="1:9" s="109" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A6" s="108"/>
-      <c r="B6" s="110" t="s">
-        <v>199</v>
-      </c>
-      <c r="C6" s="111" t="s">
-        <v>200</v>
-      </c>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
-      <c r="G6" s="112"/>
-      <c r="H6" s="112"/>
-      <c r="I6" s="107"/>
-    </row>
-    <row r="7" spans="1:9" s="109" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A7" s="108"/>
-      <c r="B7" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="C7" s="111" t="s">
-        <v>201</v>
-      </c>
-      <c r="D7" s="112"/>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="107"/>
-    </row>
-    <row r="8" spans="1:9" s="109" customFormat="1" ht="45.6" x14ac:dyDescent="0.5">
-      <c r="A8" s="108"/>
-      <c r="B8" s="110" t="s">
-        <v>172</v>
-      </c>
-      <c r="C8" s="111" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" s="135"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="107"/>
-    </row>
-    <row r="9" spans="1:9" s="130" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A9" s="126" t="s">
+      <c r="C10" s="118" t="s">
         <v>175</v>
       </c>
-      <c r="B9" s="127"/>
-      <c r="C9" s="128" t="s">
+      <c r="D10" s="122"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="119"/>
+    </row>
+    <row r="11" spans="1:9" s="120" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
+      <c r="A11" s="117"/>
+      <c r="B11" s="121" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="118" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="135"/>
+      <c r="E11" s="136"/>
+      <c r="F11" s="136"/>
+      <c r="G11" s="136"/>
+      <c r="H11" s="123"/>
+      <c r="I11" s="119"/>
+    </row>
+    <row r="12" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="117"/>
+      <c r="B12" s="121" t="s">
         <v>177</v>
       </c>
-      <c r="D9" s="129"/>
-      <c r="E9" s="129"/>
-      <c r="F9" s="129"/>
-      <c r="G9" s="129"/>
-      <c r="H9" s="129"/>
-      <c r="I9" s="129"/>
-    </row>
-    <row r="10" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="118"/>
-      <c r="B10" s="122" t="s">
-        <v>176</v>
-      </c>
-      <c r="C10" s="119" t="s">
+      <c r="C12" s="118"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="123"/>
+      <c r="F12" s="123"/>
+      <c r="G12" s="123"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="119"/>
+    </row>
+    <row r="13" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="117"/>
+      <c r="B13" s="121" t="s">
         <v>178</v>
       </c>
-      <c r="D10" s="123"/>
-      <c r="E10" s="124"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="120"/>
-    </row>
-    <row r="11" spans="1:9" s="121" customFormat="1" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A11" s="118"/>
-      <c r="B11" s="122" t="s">
+      <c r="C13" s="118"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="123"/>
+      <c r="F13" s="123"/>
+      <c r="G13" s="123"/>
+      <c r="H13" s="123"/>
+      <c r="I13" s="119"/>
+    </row>
+    <row r="14" spans="1:9" s="120" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
+      <c r="A14" s="117"/>
+      <c r="B14" s="124" t="s">
         <v>179</v>
       </c>
-      <c r="C11" s="119" t="s">
+      <c r="C14" s="118"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="123"/>
+      <c r="F14" s="123"/>
+      <c r="G14" s="123"/>
+      <c r="H14" s="123"/>
+      <c r="I14" s="119"/>
+    </row>
+    <row r="15" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="117"/>
+      <c r="B15" s="121" t="s">
+        <v>180</v>
+      </c>
+      <c r="C15" s="118"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="123"/>
+      <c r="F15" s="123"/>
+      <c r="G15" s="123"/>
+      <c r="H15" s="123"/>
+      <c r="I15" s="119"/>
+    </row>
+    <row r="16" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="117"/>
+      <c r="B16" s="121" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="118"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="123"/>
+      <c r="F16" s="123"/>
+      <c r="G16" s="123"/>
+      <c r="H16" s="123"/>
+      <c r="I16" s="119"/>
+    </row>
+    <row r="17" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="117"/>
+      <c r="B17" s="121" t="s">
+        <v>183</v>
+      </c>
+      <c r="C17" s="118" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="136"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="120"/>
-    </row>
-    <row r="12" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="118"/>
-      <c r="B12" s="122" t="s">
-        <v>180</v>
-      </c>
-      <c r="C12" s="119"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="120"/>
-    </row>
-    <row r="13" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="118"/>
-      <c r="B13" s="122" t="s">
-        <v>181</v>
-      </c>
-      <c r="C13" s="119"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="120"/>
-    </row>
-    <row r="14" spans="1:9" s="121" customFormat="1" ht="39.6" x14ac:dyDescent="0.5">
-      <c r="A14" s="118"/>
-      <c r="B14" s="125" t="s">
-        <v>182</v>
-      </c>
-      <c r="C14" s="119"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="124"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="120"/>
-    </row>
-    <row r="15" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="118"/>
-      <c r="B15" s="122" t="s">
-        <v>183</v>
-      </c>
-      <c r="C15" s="119"/>
-      <c r="D15" s="123"/>
-      <c r="E15" s="124"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="120"/>
-    </row>
-    <row r="16" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="118"/>
-      <c r="B16" s="122" t="s">
+      <c r="D17" s="130"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="131"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="119"/>
+    </row>
+    <row r="18" spans="1:9" s="120" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="117"/>
+      <c r="B18" s="121" t="s">
         <v>184</v>
       </c>
-      <c r="C16" s="119"/>
-      <c r="D16" s="123"/>
-      <c r="E16" s="124"/>
-      <c r="F16" s="124"/>
-      <c r="G16" s="124"/>
-      <c r="H16" s="124"/>
-      <c r="I16" s="120"/>
-    </row>
-    <row r="17" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="118"/>
-      <c r="B17" s="122" t="s">
+      <c r="C18" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C17" s="119" t="s">
-        <v>188</v>
-      </c>
-      <c r="D17" s="131"/>
-      <c r="E17" s="132"/>
-      <c r="F17" s="132"/>
-      <c r="G17" s="132"/>
-      <c r="H17" s="132"/>
-      <c r="I17" s="120"/>
-    </row>
-    <row r="18" spans="1:9" s="121" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="118"/>
-      <c r="B18" s="122" t="s">
-        <v>187</v>
-      </c>
-      <c r="C18" s="119" t="s">
-        <v>189</v>
-      </c>
-      <c r="D18" s="133"/>
-      <c r="E18" s="134"/>
-      <c r="F18" s="134"/>
-      <c r="G18" s="132"/>
-      <c r="H18" s="132"/>
-      <c r="I18" s="120"/>
+      <c r="D18" s="132"/>
+      <c r="E18" s="133"/>
+      <c r="F18" s="133"/>
+      <c r="G18" s="131"/>
+      <c r="H18" s="131"/>
+      <c r="I18" s="119"/>
     </row>
     <row r="19" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="20" spans="1:9" customFormat="1" ht="14.4" x14ac:dyDescent="0.3"/>
@@ -3713,48 +3795,48 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E1" t="s">
         <v>62</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G1" t="s">
         <v>74</v>
       </c>
       <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1" t="s">
+        <v>128</v>
+      </c>
+      <c r="L1" t="s">
         <v>129</v>
       </c>
-      <c r="I1" t="s">
-        <v>83</v>
-      </c>
-      <c r="J1" t="s">
-        <v>130</v>
-      </c>
-      <c r="K1" t="s">
-        <v>131</v>
-      </c>
-      <c r="L1" t="s">
-        <v>132</v>
-      </c>
       <c r="M1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="N1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -3763,48 +3845,48 @@
         <v>29</v>
       </c>
       <c r="E2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" t="s">
         <v>135</v>
       </c>
-      <c r="F2" t="s">
+      <c r="K2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" t="s">
         <v>136</v>
       </c>
-      <c r="G2" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" t="s">
-        <v>136</v>
-      </c>
-      <c r="I2" t="s">
-        <v>136</v>
-      </c>
-      <c r="J2" t="s">
-        <v>138</v>
-      </c>
-      <c r="K2" t="s">
-        <v>93</v>
-      </c>
-      <c r="L2" t="s">
-        <v>139</v>
-      </c>
       <c r="M2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="N2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
         <v>64</v>
@@ -3813,7 +3895,7 @@
         <v>73</v>
       </c>
       <c r="G3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H3" t="s">
         <v>73</v>
@@ -3822,98 +3904,98 @@
         <v>73</v>
       </c>
       <c r="J3" t="s">
+        <v>140</v>
+      </c>
+      <c r="K3" t="s">
+        <v>141</v>
+      </c>
+      <c r="L3" t="s">
+        <v>142</v>
+      </c>
+      <c r="M3" t="s">
         <v>143</v>
       </c>
-      <c r="K3" t="s">
-        <v>144</v>
-      </c>
-      <c r="L3" t="s">
-        <v>145</v>
-      </c>
-      <c r="M3" t="s">
-        <v>146</v>
-      </c>
       <c r="N3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" t="s">
         <v>147</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>148</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
         <v>149</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
+        <v>145</v>
+      </c>
+      <c r="I4" t="s">
         <v>150</v>
       </c>
-      <c r="E4" t="s">
+      <c r="J4" t="s">
         <v>151</v>
       </c>
-      <c r="F4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="K4" t="s">
         <v>152</v>
       </c>
-      <c r="H4" t="s">
-        <v>148</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>153</v>
       </c>
-      <c r="J4" t="s">
+      <c r="M4" t="s">
         <v>154</v>
       </c>
-      <c r="K4" t="s">
-        <v>155</v>
-      </c>
-      <c r="L4" t="s">
-        <v>156</v>
-      </c>
-      <c r="M4" t="s">
-        <v>157</v>
-      </c>
       <c r="N4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" t="s">
+        <v>79</v>
+      </c>
+      <c r="I5" t="s">
+        <v>145</v>
+      </c>
+      <c r="J5" t="s">
+        <v>97</v>
+      </c>
+      <c r="L5" t="s">
         <v>158</v>
       </c>
-      <c r="B5" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" t="s">
-        <v>160</v>
-      </c>
-      <c r="F5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" t="s">
-        <v>148</v>
-      </c>
-      <c r="J5" t="s">
-        <v>100</v>
-      </c>
-      <c r="L5" t="s">
-        <v>161</v>
-      </c>
       <c r="N5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -3921,36 +4003,36 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
+        <v>159</v>
+      </c>
+      <c r="I6" t="s">
+        <v>160</v>
+      </c>
+      <c r="J6" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" t="s">
         <v>162</v>
       </c>
-      <c r="I6" t="s">
-        <v>163</v>
-      </c>
-      <c r="J6" t="s">
-        <v>164</v>
-      </c>
-      <c r="L6" t="s">
-        <v>165</v>
-      </c>
       <c r="N6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="J7" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="L7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3960,65 +4042,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
+      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
+      <Description>YVWEJ5DVYS2U-421999773-68</Description>
+    </_dlc_DocIdUrl>
+    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008D4902BA52C7D94A994657A564808B2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e4455a60d2ff5f5fcd8815d6d89b5b66">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b541edd5-2552-480e-ada6-0e2c8d317108" xmlns:ns3="780ae317-08c5-4e10-af93-dd385a8384a9" xmlns:ns4="3146657c-56f4-4c0a-bb9c-a675121ac670" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1d01ecd782f081d5d944fa263943fc4" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="b541edd5-2552-480e-ada6-0e2c8d317108"/>
@@ -4217,37 +4254,84 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">YVWEJ5DVYS2U-421999773-68</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="b541edd5-2552-480e-ada6-0e2c8d317108">
-      <Url>https://cdcpartners.sharepoint.com/sites/NCHS/nvssmodcop/_layouts/15/DocIdRedir.aspx?ID=YVWEJ5DVYS2U-421999773-68</Url>
-      <Description>YVWEJ5DVYS2U-421999773-68</Description>
-    </_dlc_DocIdUrl>
-    <ShareFileCreator xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-    <ShareFileCreated xmlns="780ae317-08c5-4e10-af93-dd385a8384a9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0980278E-2A79-4F44-8623-FE545C304BE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4267,20 +4351,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CF0D7A6D-D78F-4048-9348-0B4289842B11}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69E3EF86-6C9E-4C22-A476-13DA012C68C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{448710E8-BE9E-4C9E-A40A-0AC1DAE48E99}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="780ae317-08c5-4e10-af93-dd385a8384a9"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b541edd5-2552-480e-ada6-0e2c8d317108"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3146657c-56f4-4c0a-bb9c-a675121ac670"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>